<commit_message>
test excel with non null values, fix lists and lists of lists handling, improve dictionary handling, make all embedding vectors lists not dicts
</commit_message>
<xml_diff>
--- a/excel_sheets/Document_metadata.xlsx
+++ b/excel_sheets/Document_metadata.xlsx
@@ -4259,9 +4259,7 @@
           <t>url</t>
         </is>
       </c>
-      <c r="C32" s="6" t="n">
-        <v/>
-      </c>
+      <c r="C32" s="6" t="n"/>
       <c r="D32" s="6" t="n"/>
       <c r="E32" s="6" t="n"/>
       <c r="F32" s="6" t="n"/>
@@ -13730,10 +13728,8 @@
           <t>id</t>
         </is>
       </c>
-      <c r="C2" s="5" t="n">
-        <v/>
-      </c>
-      <c r="D2" s="6" t="inlineStr"/>
+      <c r="C2" s="6" t="inlineStr"/>
+      <c r="D2" s="6" t="n"/>
       <c r="E2" s="6" t="n"/>
       <c r="F2" s="6" t="n"/>
       <c r="G2" s="6" t="n"/>
@@ -13768,9 +13764,7 @@
           <t>description</t>
         </is>
       </c>
-      <c r="C3" s="5" t="n">
-        <v/>
-      </c>
+      <c r="C3" s="6" t="n"/>
       <c r="D3" s="6" t="n"/>
       <c r="E3" s="6" t="n"/>
       <c r="F3" s="6" t="n"/>
@@ -13806,9 +13800,7 @@
           <t>date</t>
         </is>
       </c>
-      <c r="C4" s="5" t="n">
-        <v/>
-      </c>
+      <c r="C4" s="6" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
       <c r="F4" s="6" t="n"/>
@@ -13844,8 +13836,12 @@
           <t>vector</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="inlineStr"/>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>[""]</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="n"/>
       <c r="E5" s="6" t="n"/>
       <c r="F5" s="6" t="n"/>
       <c r="G5" s="6" t="n"/>
@@ -13876,7 +13872,7 @@
     <row r="6">
       <c r="A6" s="4" t="n"/>
       <c r="B6" s="8" t="n"/>
-      <c r="C6" s="8" t="n"/>
+      <c r="C6" s="2" t="n"/>
       <c r="D6" s="2" t="n"/>
       <c r="E6" s="2" t="n"/>
       <c r="F6" s="2" t="n"/>

</xml_diff>

<commit_message>
remove LDA and Embeddings from schemas
</commit_message>
<xml_diff>
--- a/excel_sheets/Document_metadata.xlsx
+++ b/excel_sheets/Document_metadata.xlsx
@@ -12,8 +12,6 @@
     <sheet name="document_description" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="provenance" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="tags" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="lda_topics" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="embeddings" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -12531,2338 +12529,4 @@
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AD34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>lda_topics</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr"/>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>model_info</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>[{"source": null, "author": null, "version": null, "model_id": null, "nb_topics": null, "description": null, "corpus": null, "uri": null}]</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="n"/>
-      <c r="E2" s="6" t="n"/>
-      <c r="F2" s="6" t="n"/>
-      <c r="G2" s="6" t="n"/>
-      <c r="H2" s="6" t="n"/>
-      <c r="I2" s="6" t="n"/>
-      <c r="J2" s="6" t="n"/>
-      <c r="K2" s="6" t="n"/>
-      <c r="L2" s="6" t="n"/>
-      <c r="M2" s="6" t="n"/>
-      <c r="N2" s="6" t="n"/>
-      <c r="O2" s="6" t="n"/>
-      <c r="P2" s="6" t="n"/>
-      <c r="Q2" s="6" t="n"/>
-      <c r="R2" s="6" t="n"/>
-      <c r="S2" s="6" t="n"/>
-      <c r="T2" s="6" t="n"/>
-      <c r="U2" s="6" t="n"/>
-      <c r="V2" s="6" t="n"/>
-      <c r="W2" s="6" t="n"/>
-      <c r="X2" s="6" t="n"/>
-      <c r="Y2" s="6" t="n"/>
-      <c r="Z2" s="6" t="n"/>
-      <c r="AA2" s="6" t="n"/>
-      <c r="AB2" s="6" t="n"/>
-      <c r="AC2" s="6" t="n"/>
-      <c r="AD2" s="6" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr"/>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>topic_description</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[{"topic_id": null, "topic_score": null, "topic_label": null, "topic_words": [{"word": null, "word_weight": null}]}]</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="n"/>
-      <c r="G3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="6" t="n"/>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="6" t="n"/>
-      <c r="L3" s="6" t="n"/>
-      <c r="M3" s="6" t="n"/>
-      <c r="N3" s="6" t="n"/>
-      <c r="O3" s="6" t="n"/>
-      <c r="P3" s="6" t="n"/>
-      <c r="Q3" s="6" t="n"/>
-      <c r="R3" s="6" t="n"/>
-      <c r="S3" s="6" t="n"/>
-      <c r="T3" s="6" t="n"/>
-      <c r="U3" s="6" t="n"/>
-      <c r="V3" s="6" t="n"/>
-      <c r="W3" s="6" t="n"/>
-      <c r="X3" s="6" t="n"/>
-      <c r="Y3" s="6" t="n"/>
-      <c r="Z3" s="6" t="n"/>
-      <c r="AA3" s="6" t="n"/>
-      <c r="AB3" s="6" t="n"/>
-      <c r="AC3" s="6" t="n"/>
-      <c r="AD3" s="6" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="n"/>
-      <c r="B4" s="8" t="n"/>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
-      <c r="K4" s="2" t="n"/>
-      <c r="L4" s="2" t="n"/>
-      <c r="M4" s="2" t="n"/>
-      <c r="N4" s="2" t="n"/>
-      <c r="O4" s="2" t="n"/>
-      <c r="P4" s="2" t="n"/>
-      <c r="Q4" s="2" t="n"/>
-      <c r="R4" s="2" t="n"/>
-      <c r="S4" s="2" t="n"/>
-      <c r="T4" s="2" t="n"/>
-      <c r="U4" s="2" t="n"/>
-      <c r="V4" s="2" t="n"/>
-      <c r="W4" s="2" t="n"/>
-      <c r="X4" s="2" t="n"/>
-      <c r="Y4" s="2" t="n"/>
-      <c r="Z4" s="2" t="n"/>
-      <c r="AA4" s="2" t="n"/>
-      <c r="AB4" s="2" t="n"/>
-      <c r="AC4" s="2" t="n"/>
-      <c r="AD4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="n"/>
-      <c r="B5" s="4" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="4" t="n"/>
-      <c r="E5" s="4" t="n"/>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="4" t="n"/>
-      <c r="H5" s="4" t="n"/>
-      <c r="I5" s="4" t="n"/>
-      <c r="J5" s="4" t="n"/>
-      <c r="K5" s="4" t="n"/>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="4" t="n"/>
-      <c r="N5" s="4" t="n"/>
-      <c r="O5" s="4" t="n"/>
-      <c r="P5" s="4" t="n"/>
-      <c r="Q5" s="4" t="n"/>
-      <c r="R5" s="4" t="n"/>
-      <c r="S5" s="4" t="n"/>
-      <c r="T5" s="4" t="n"/>
-      <c r="U5" s="4" t="n"/>
-      <c r="V5" s="4" t="n"/>
-      <c r="W5" s="4" t="n"/>
-      <c r="X5" s="4" t="n"/>
-      <c r="Y5" s="4" t="n"/>
-      <c r="Z5" s="4" t="n"/>
-      <c r="AA5" s="4" t="n"/>
-      <c r="AB5" s="4" t="n"/>
-      <c r="AC5" s="4" t="n"/>
-      <c r="AD5" s="4" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="4" t="n"/>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="4" t="n"/>
-      <c r="E6" s="4" t="n"/>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="4" t="n"/>
-      <c r="H6" s="4" t="n"/>
-      <c r="I6" s="4" t="n"/>
-      <c r="J6" s="4" t="n"/>
-      <c r="K6" s="4" t="n"/>
-      <c r="L6" s="4" t="n"/>
-      <c r="M6" s="4" t="n"/>
-      <c r="N6" s="4" t="n"/>
-      <c r="O6" s="4" t="n"/>
-      <c r="P6" s="4" t="n"/>
-      <c r="Q6" s="4" t="n"/>
-      <c r="R6" s="4" t="n"/>
-      <c r="S6" s="4" t="n"/>
-      <c r="T6" s="4" t="n"/>
-      <c r="U6" s="4" t="n"/>
-      <c r="V6" s="4" t="n"/>
-      <c r="W6" s="4" t="n"/>
-      <c r="X6" s="4" t="n"/>
-      <c r="Y6" s="4" t="n"/>
-      <c r="Z6" s="4" t="n"/>
-      <c r="AA6" s="4" t="n"/>
-      <c r="AB6" s="4" t="n"/>
-      <c r="AC6" s="4" t="n"/>
-      <c r="AD6" s="4" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n"/>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="4" t="n"/>
-      <c r="E7" s="4" t="n"/>
-      <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
-      <c r="H7" s="4" t="n"/>
-      <c r="I7" s="4" t="n"/>
-      <c r="J7" s="4" t="n"/>
-      <c r="K7" s="4" t="n"/>
-      <c r="L7" s="4" t="n"/>
-      <c r="M7" s="4" t="n"/>
-      <c r="N7" s="4" t="n"/>
-      <c r="O7" s="4" t="n"/>
-      <c r="P7" s="4" t="n"/>
-      <c r="Q7" s="4" t="n"/>
-      <c r="R7" s="4" t="n"/>
-      <c r="S7" s="4" t="n"/>
-      <c r="T7" s="4" t="n"/>
-      <c r="U7" s="4" t="n"/>
-      <c r="V7" s="4" t="n"/>
-      <c r="W7" s="4" t="n"/>
-      <c r="X7" s="4" t="n"/>
-      <c r="Y7" s="4" t="n"/>
-      <c r="Z7" s="4" t="n"/>
-      <c r="AA7" s="4" t="n"/>
-      <c r="AB7" s="4" t="n"/>
-      <c r="AC7" s="4" t="n"/>
-      <c r="AD7" s="4" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="4" t="n"/>
-      <c r="E8" s="4" t="n"/>
-      <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
-      <c r="H8" s="4" t="n"/>
-      <c r="I8" s="4" t="n"/>
-      <c r="J8" s="4" t="n"/>
-      <c r="K8" s="4" t="n"/>
-      <c r="L8" s="4" t="n"/>
-      <c r="M8" s="4" t="n"/>
-      <c r="N8" s="4" t="n"/>
-      <c r="O8" s="4" t="n"/>
-      <c r="P8" s="4" t="n"/>
-      <c r="Q8" s="4" t="n"/>
-      <c r="R8" s="4" t="n"/>
-      <c r="S8" s="4" t="n"/>
-      <c r="T8" s="4" t="n"/>
-      <c r="U8" s="4" t="n"/>
-      <c r="V8" s="4" t="n"/>
-      <c r="W8" s="4" t="n"/>
-      <c r="X8" s="4" t="n"/>
-      <c r="Y8" s="4" t="n"/>
-      <c r="Z8" s="4" t="n"/>
-      <c r="AA8" s="4" t="n"/>
-      <c r="AB8" s="4" t="n"/>
-      <c r="AC8" s="4" t="n"/>
-      <c r="AD8" s="4" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n"/>
-      <c r="B9" s="4" t="n"/>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="4" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
-      <c r="H9" s="4" t="n"/>
-      <c r="I9" s="4" t="n"/>
-      <c r="J9" s="4" t="n"/>
-      <c r="K9" s="4" t="n"/>
-      <c r="L9" s="4" t="n"/>
-      <c r="M9" s="4" t="n"/>
-      <c r="N9" s="4" t="n"/>
-      <c r="O9" s="4" t="n"/>
-      <c r="P9" s="4" t="n"/>
-      <c r="Q9" s="4" t="n"/>
-      <c r="R9" s="4" t="n"/>
-      <c r="S9" s="4" t="n"/>
-      <c r="T9" s="4" t="n"/>
-      <c r="U9" s="4" t="n"/>
-      <c r="V9" s="4" t="n"/>
-      <c r="W9" s="4" t="n"/>
-      <c r="X9" s="4" t="n"/>
-      <c r="Y9" s="4" t="n"/>
-      <c r="Z9" s="4" t="n"/>
-      <c r="AA9" s="4" t="n"/>
-      <c r="AB9" s="4" t="n"/>
-      <c r="AC9" s="4" t="n"/>
-      <c r="AD9" s="4" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n"/>
-      <c r="B10" s="4" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="4" t="n"/>
-      <c r="E10" s="4" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="4" t="n"/>
-      <c r="H10" s="4" t="n"/>
-      <c r="I10" s="4" t="n"/>
-      <c r="J10" s="4" t="n"/>
-      <c r="K10" s="4" t="n"/>
-      <c r="L10" s="4" t="n"/>
-      <c r="M10" s="4" t="n"/>
-      <c r="N10" s="4" t="n"/>
-      <c r="O10" s="4" t="n"/>
-      <c r="P10" s="4" t="n"/>
-      <c r="Q10" s="4" t="n"/>
-      <c r="R10" s="4" t="n"/>
-      <c r="S10" s="4" t="n"/>
-      <c r="T10" s="4" t="n"/>
-      <c r="U10" s="4" t="n"/>
-      <c r="V10" s="4" t="n"/>
-      <c r="W10" s="4" t="n"/>
-      <c r="X10" s="4" t="n"/>
-      <c r="Y10" s="4" t="n"/>
-      <c r="Z10" s="4" t="n"/>
-      <c r="AA10" s="4" t="n"/>
-      <c r="AB10" s="4" t="n"/>
-      <c r="AC10" s="4" t="n"/>
-      <c r="AD10" s="4" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="4" t="n"/>
-      <c r="D11" s="4" t="n"/>
-      <c r="E11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="n"/>
-      <c r="H11" s="4" t="n"/>
-      <c r="I11" s="4" t="n"/>
-      <c r="J11" s="4" t="n"/>
-      <c r="K11" s="4" t="n"/>
-      <c r="L11" s="4" t="n"/>
-      <c r="M11" s="4" t="n"/>
-      <c r="N11" s="4" t="n"/>
-      <c r="O11" s="4" t="n"/>
-      <c r="P11" s="4" t="n"/>
-      <c r="Q11" s="4" t="n"/>
-      <c r="R11" s="4" t="n"/>
-      <c r="S11" s="4" t="n"/>
-      <c r="T11" s="4" t="n"/>
-      <c r="U11" s="4" t="n"/>
-      <c r="V11" s="4" t="n"/>
-      <c r="W11" s="4" t="n"/>
-      <c r="X11" s="4" t="n"/>
-      <c r="Y11" s="4" t="n"/>
-      <c r="Z11" s="4" t="n"/>
-      <c r="AA11" s="4" t="n"/>
-      <c r="AB11" s="4" t="n"/>
-      <c r="AC11" s="4" t="n"/>
-      <c r="AD11" s="4" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="4" t="n"/>
-      <c r="J12" s="4" t="n"/>
-      <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
-      <c r="N12" s="4" t="n"/>
-      <c r="O12" s="4" t="n"/>
-      <c r="P12" s="4" t="n"/>
-      <c r="Q12" s="4" t="n"/>
-      <c r="R12" s="4" t="n"/>
-      <c r="S12" s="4" t="n"/>
-      <c r="T12" s="4" t="n"/>
-      <c r="U12" s="4" t="n"/>
-      <c r="V12" s="4" t="n"/>
-      <c r="W12" s="4" t="n"/>
-      <c r="X12" s="4" t="n"/>
-      <c r="Y12" s="4" t="n"/>
-      <c r="Z12" s="4" t="n"/>
-      <c r="AA12" s="4" t="n"/>
-      <c r="AB12" s="4" t="n"/>
-      <c r="AC12" s="4" t="n"/>
-      <c r="AD12" s="4" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n"/>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" s="4" t="n"/>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
-      <c r="H13" s="4" t="n"/>
-      <c r="I13" s="4" t="n"/>
-      <c r="J13" s="4" t="n"/>
-      <c r="K13" s="4" t="n"/>
-      <c r="L13" s="4" t="n"/>
-      <c r="M13" s="4" t="n"/>
-      <c r="N13" s="4" t="n"/>
-      <c r="O13" s="4" t="n"/>
-      <c r="P13" s="4" t="n"/>
-      <c r="Q13" s="4" t="n"/>
-      <c r="R13" s="4" t="n"/>
-      <c r="S13" s="4" t="n"/>
-      <c r="T13" s="4" t="n"/>
-      <c r="U13" s="4" t="n"/>
-      <c r="V13" s="4" t="n"/>
-      <c r="W13" s="4" t="n"/>
-      <c r="X13" s="4" t="n"/>
-      <c r="Y13" s="4" t="n"/>
-      <c r="Z13" s="4" t="n"/>
-      <c r="AA13" s="4" t="n"/>
-      <c r="AB13" s="4" t="n"/>
-      <c r="AC13" s="4" t="n"/>
-      <c r="AD13" s="4" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n"/>
-      <c r="B14" s="4" t="n"/>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="4" t="n"/>
-      <c r="E14" s="4" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="4" t="n"/>
-      <c r="I14" s="4" t="n"/>
-      <c r="J14" s="4" t="n"/>
-      <c r="K14" s="4" t="n"/>
-      <c r="L14" s="4" t="n"/>
-      <c r="M14" s="4" t="n"/>
-      <c r="N14" s="4" t="n"/>
-      <c r="O14" s="4" t="n"/>
-      <c r="P14" s="4" t="n"/>
-      <c r="Q14" s="4" t="n"/>
-      <c r="R14" s="4" t="n"/>
-      <c r="S14" s="4" t="n"/>
-      <c r="T14" s="4" t="n"/>
-      <c r="U14" s="4" t="n"/>
-      <c r="V14" s="4" t="n"/>
-      <c r="W14" s="4" t="n"/>
-      <c r="X14" s="4" t="n"/>
-      <c r="Y14" s="4" t="n"/>
-      <c r="Z14" s="4" t="n"/>
-      <c r="AA14" s="4" t="n"/>
-      <c r="AB14" s="4" t="n"/>
-      <c r="AC14" s="4" t="n"/>
-      <c r="AD14" s="4" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n"/>
-      <c r="B15" s="4" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="4" t="n"/>
-      <c r="E15" s="4" t="n"/>
-      <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="n"/>
-      <c r="H15" s="4" t="n"/>
-      <c r="I15" s="4" t="n"/>
-      <c r="J15" s="4" t="n"/>
-      <c r="K15" s="4" t="n"/>
-      <c r="L15" s="4" t="n"/>
-      <c r="M15" s="4" t="n"/>
-      <c r="N15" s="4" t="n"/>
-      <c r="O15" s="4" t="n"/>
-      <c r="P15" s="4" t="n"/>
-      <c r="Q15" s="4" t="n"/>
-      <c r="R15" s="4" t="n"/>
-      <c r="S15" s="4" t="n"/>
-      <c r="T15" s="4" t="n"/>
-      <c r="U15" s="4" t="n"/>
-      <c r="V15" s="4" t="n"/>
-      <c r="W15" s="4" t="n"/>
-      <c r="X15" s="4" t="n"/>
-      <c r="Y15" s="4" t="n"/>
-      <c r="Z15" s="4" t="n"/>
-      <c r="AA15" s="4" t="n"/>
-      <c r="AB15" s="4" t="n"/>
-      <c r="AC15" s="4" t="n"/>
-      <c r="AD15" s="4" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n"/>
-      <c r="B16" s="4" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="4" t="n"/>
-      <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="n"/>
-      <c r="H16" s="4" t="n"/>
-      <c r="I16" s="4" t="n"/>
-      <c r="J16" s="4" t="n"/>
-      <c r="K16" s="4" t="n"/>
-      <c r="L16" s="4" t="n"/>
-      <c r="M16" s="4" t="n"/>
-      <c r="N16" s="4" t="n"/>
-      <c r="O16" s="4" t="n"/>
-      <c r="P16" s="4" t="n"/>
-      <c r="Q16" s="4" t="n"/>
-      <c r="R16" s="4" t="n"/>
-      <c r="S16" s="4" t="n"/>
-      <c r="T16" s="4" t="n"/>
-      <c r="U16" s="4" t="n"/>
-      <c r="V16" s="4" t="n"/>
-      <c r="W16" s="4" t="n"/>
-      <c r="X16" s="4" t="n"/>
-      <c r="Y16" s="4" t="n"/>
-      <c r="Z16" s="4" t="n"/>
-      <c r="AA16" s="4" t="n"/>
-      <c r="AB16" s="4" t="n"/>
-      <c r="AC16" s="4" t="n"/>
-      <c r="AD16" s="4" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n"/>
-      <c r="B17" s="4" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="4" t="n"/>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
-      <c r="G17" s="4" t="n"/>
-      <c r="H17" s="4" t="n"/>
-      <c r="I17" s="4" t="n"/>
-      <c r="J17" s="4" t="n"/>
-      <c r="K17" s="4" t="n"/>
-      <c r="L17" s="4" t="n"/>
-      <c r="M17" s="4" t="n"/>
-      <c r="N17" s="4" t="n"/>
-      <c r="O17" s="4" t="n"/>
-      <c r="P17" s="4" t="n"/>
-      <c r="Q17" s="4" t="n"/>
-      <c r="R17" s="4" t="n"/>
-      <c r="S17" s="4" t="n"/>
-      <c r="T17" s="4" t="n"/>
-      <c r="U17" s="4" t="n"/>
-      <c r="V17" s="4" t="n"/>
-      <c r="W17" s="4" t="n"/>
-      <c r="X17" s="4" t="n"/>
-      <c r="Y17" s="4" t="n"/>
-      <c r="Z17" s="4" t="n"/>
-      <c r="AA17" s="4" t="n"/>
-      <c r="AB17" s="4" t="n"/>
-      <c r="AC17" s="4" t="n"/>
-      <c r="AD17" s="4" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="4" t="n"/>
-      <c r="F18" s="4" t="n"/>
-      <c r="G18" s="4" t="n"/>
-      <c r="H18" s="4" t="n"/>
-      <c r="I18" s="4" t="n"/>
-      <c r="J18" s="4" t="n"/>
-      <c r="K18" s="4" t="n"/>
-      <c r="L18" s="4" t="n"/>
-      <c r="M18" s="4" t="n"/>
-      <c r="N18" s="4" t="n"/>
-      <c r="O18" s="4" t="n"/>
-      <c r="P18" s="4" t="n"/>
-      <c r="Q18" s="4" t="n"/>
-      <c r="R18" s="4" t="n"/>
-      <c r="S18" s="4" t="n"/>
-      <c r="T18" s="4" t="n"/>
-      <c r="U18" s="4" t="n"/>
-      <c r="V18" s="4" t="n"/>
-      <c r="W18" s="4" t="n"/>
-      <c r="X18" s="4" t="n"/>
-      <c r="Y18" s="4" t="n"/>
-      <c r="Z18" s="4" t="n"/>
-      <c r="AA18" s="4" t="n"/>
-      <c r="AB18" s="4" t="n"/>
-      <c r="AC18" s="4" t="n"/>
-      <c r="AD18" s="4" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="n"/>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="4" t="n"/>
-      <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="4" t="n"/>
-      <c r="I19" s="4" t="n"/>
-      <c r="J19" s="4" t="n"/>
-      <c r="K19" s="4" t="n"/>
-      <c r="L19" s="4" t="n"/>
-      <c r="M19" s="4" t="n"/>
-      <c r="N19" s="4" t="n"/>
-      <c r="O19" s="4" t="n"/>
-      <c r="P19" s="4" t="n"/>
-      <c r="Q19" s="4" t="n"/>
-      <c r="R19" s="4" t="n"/>
-      <c r="S19" s="4" t="n"/>
-      <c r="T19" s="4" t="n"/>
-      <c r="U19" s="4" t="n"/>
-      <c r="V19" s="4" t="n"/>
-      <c r="W19" s="4" t="n"/>
-      <c r="X19" s="4" t="n"/>
-      <c r="Y19" s="4" t="n"/>
-      <c r="Z19" s="4" t="n"/>
-      <c r="AA19" s="4" t="n"/>
-      <c r="AB19" s="4" t="n"/>
-      <c r="AC19" s="4" t="n"/>
-      <c r="AD19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="4" t="n"/>
-      <c r="E20" s="4" t="n"/>
-      <c r="F20" s="4" t="n"/>
-      <c r="G20" s="4" t="n"/>
-      <c r="H20" s="4" t="n"/>
-      <c r="I20" s="4" t="n"/>
-      <c r="J20" s="4" t="n"/>
-      <c r="K20" s="4" t="n"/>
-      <c r="L20" s="4" t="n"/>
-      <c r="M20" s="4" t="n"/>
-      <c r="N20" s="4" t="n"/>
-      <c r="O20" s="4" t="n"/>
-      <c r="P20" s="4" t="n"/>
-      <c r="Q20" s="4" t="n"/>
-      <c r="R20" s="4" t="n"/>
-      <c r="S20" s="4" t="n"/>
-      <c r="T20" s="4" t="n"/>
-      <c r="U20" s="4" t="n"/>
-      <c r="V20" s="4" t="n"/>
-      <c r="W20" s="4" t="n"/>
-      <c r="X20" s="4" t="n"/>
-      <c r="Y20" s="4" t="n"/>
-      <c r="Z20" s="4" t="n"/>
-      <c r="AA20" s="4" t="n"/>
-      <c r="AB20" s="4" t="n"/>
-      <c r="AC20" s="4" t="n"/>
-      <c r="AD20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="n"/>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
-      <c r="G21" s="4" t="n"/>
-      <c r="H21" s="4" t="n"/>
-      <c r="I21" s="4" t="n"/>
-      <c r="J21" s="4" t="n"/>
-      <c r="K21" s="4" t="n"/>
-      <c r="L21" s="4" t="n"/>
-      <c r="M21" s="4" t="n"/>
-      <c r="N21" s="4" t="n"/>
-      <c r="O21" s="4" t="n"/>
-      <c r="P21" s="4" t="n"/>
-      <c r="Q21" s="4" t="n"/>
-      <c r="R21" s="4" t="n"/>
-      <c r="S21" s="4" t="n"/>
-      <c r="T21" s="4" t="n"/>
-      <c r="U21" s="4" t="n"/>
-      <c r="V21" s="4" t="n"/>
-      <c r="W21" s="4" t="n"/>
-      <c r="X21" s="4" t="n"/>
-      <c r="Y21" s="4" t="n"/>
-      <c r="Z21" s="4" t="n"/>
-      <c r="AA21" s="4" t="n"/>
-      <c r="AB21" s="4" t="n"/>
-      <c r="AC21" s="4" t="n"/>
-      <c r="AD21" s="4" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="n"/>
-      <c r="B22" s="4" t="n"/>
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
-      <c r="G22" s="4" t="n"/>
-      <c r="H22" s="4" t="n"/>
-      <c r="I22" s="4" t="n"/>
-      <c r="J22" s="4" t="n"/>
-      <c r="K22" s="4" t="n"/>
-      <c r="L22" s="4" t="n"/>
-      <c r="M22" s="4" t="n"/>
-      <c r="N22" s="4" t="n"/>
-      <c r="O22" s="4" t="n"/>
-      <c r="P22" s="4" t="n"/>
-      <c r="Q22" s="4" t="n"/>
-      <c r="R22" s="4" t="n"/>
-      <c r="S22" s="4" t="n"/>
-      <c r="T22" s="4" t="n"/>
-      <c r="U22" s="4" t="n"/>
-      <c r="V22" s="4" t="n"/>
-      <c r="W22" s="4" t="n"/>
-      <c r="X22" s="4" t="n"/>
-      <c r="Y22" s="4" t="n"/>
-      <c r="Z22" s="4" t="n"/>
-      <c r="AA22" s="4" t="n"/>
-      <c r="AB22" s="4" t="n"/>
-      <c r="AC22" s="4" t="n"/>
-      <c r="AD22" s="4" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="n"/>
-      <c r="B23" s="4" t="n"/>
-      <c r="C23" s="4" t="n"/>
-      <c r="D23" s="4" t="n"/>
-      <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
-      <c r="G23" s="4" t="n"/>
-      <c r="H23" s="4" t="n"/>
-      <c r="I23" s="4" t="n"/>
-      <c r="J23" s="4" t="n"/>
-      <c r="K23" s="4" t="n"/>
-      <c r="L23" s="4" t="n"/>
-      <c r="M23" s="4" t="n"/>
-      <c r="N23" s="4" t="n"/>
-      <c r="O23" s="4" t="n"/>
-      <c r="P23" s="4" t="n"/>
-      <c r="Q23" s="4" t="n"/>
-      <c r="R23" s="4" t="n"/>
-      <c r="S23" s="4" t="n"/>
-      <c r="T23" s="4" t="n"/>
-      <c r="U23" s="4" t="n"/>
-      <c r="V23" s="4" t="n"/>
-      <c r="W23" s="4" t="n"/>
-      <c r="X23" s="4" t="n"/>
-      <c r="Y23" s="4" t="n"/>
-      <c r="Z23" s="4" t="n"/>
-      <c r="AA23" s="4" t="n"/>
-      <c r="AB23" s="4" t="n"/>
-      <c r="AC23" s="4" t="n"/>
-      <c r="AD23" s="4" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="n"/>
-      <c r="B24" s="4" t="n"/>
-      <c r="C24" s="4" t="n"/>
-      <c r="D24" s="4" t="n"/>
-      <c r="E24" s="4" t="n"/>
-      <c r="F24" s="4" t="n"/>
-      <c r="G24" s="4" t="n"/>
-      <c r="H24" s="4" t="n"/>
-      <c r="I24" s="4" t="n"/>
-      <c r="J24" s="4" t="n"/>
-      <c r="K24" s="4" t="n"/>
-      <c r="L24" s="4" t="n"/>
-      <c r="M24" s="4" t="n"/>
-      <c r="N24" s="4" t="n"/>
-      <c r="O24" s="4" t="n"/>
-      <c r="P24" s="4" t="n"/>
-      <c r="Q24" s="4" t="n"/>
-      <c r="R24" s="4" t="n"/>
-      <c r="S24" s="4" t="n"/>
-      <c r="T24" s="4" t="n"/>
-      <c r="U24" s="4" t="n"/>
-      <c r="V24" s="4" t="n"/>
-      <c r="W24" s="4" t="n"/>
-      <c r="X24" s="4" t="n"/>
-      <c r="Y24" s="4" t="n"/>
-      <c r="Z24" s="4" t="n"/>
-      <c r="AA24" s="4" t="n"/>
-      <c r="AB24" s="4" t="n"/>
-      <c r="AC24" s="4" t="n"/>
-      <c r="AD24" s="4" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="4" t="n"/>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="4" t="n"/>
-      <c r="G25" s="4" t="n"/>
-      <c r="H25" s="4" t="n"/>
-      <c r="I25" s="4" t="n"/>
-      <c r="J25" s="4" t="n"/>
-      <c r="K25" s="4" t="n"/>
-      <c r="L25" s="4" t="n"/>
-      <c r="M25" s="4" t="n"/>
-      <c r="N25" s="4" t="n"/>
-      <c r="O25" s="4" t="n"/>
-      <c r="P25" s="4" t="n"/>
-      <c r="Q25" s="4" t="n"/>
-      <c r="R25" s="4" t="n"/>
-      <c r="S25" s="4" t="n"/>
-      <c r="T25" s="4" t="n"/>
-      <c r="U25" s="4" t="n"/>
-      <c r="V25" s="4" t="n"/>
-      <c r="W25" s="4" t="n"/>
-      <c r="X25" s="4" t="n"/>
-      <c r="Y25" s="4" t="n"/>
-      <c r="Z25" s="4" t="n"/>
-      <c r="AA25" s="4" t="n"/>
-      <c r="AB25" s="4" t="n"/>
-      <c r="AC25" s="4" t="n"/>
-      <c r="AD25" s="4" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="n"/>
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="M26" s="4" t="n"/>
-      <c r="N26" s="4" t="n"/>
-      <c r="O26" s="4" t="n"/>
-      <c r="P26" s="4" t="n"/>
-      <c r="Q26" s="4" t="n"/>
-      <c r="R26" s="4" t="n"/>
-      <c r="S26" s="4" t="n"/>
-      <c r="T26" s="4" t="n"/>
-      <c r="U26" s="4" t="n"/>
-      <c r="V26" s="4" t="n"/>
-      <c r="W26" s="4" t="n"/>
-      <c r="X26" s="4" t="n"/>
-      <c r="Y26" s="4" t="n"/>
-      <c r="Z26" s="4" t="n"/>
-      <c r="AA26" s="4" t="n"/>
-      <c r="AB26" s="4" t="n"/>
-      <c r="AC26" s="4" t="n"/>
-      <c r="AD26" s="4" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="n"/>
-      <c r="B27" s="4" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="4" t="n"/>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="4" t="n"/>
-      <c r="G27" s="4" t="n"/>
-      <c r="H27" s="4" t="n"/>
-      <c r="I27" s="4" t="n"/>
-      <c r="J27" s="4" t="n"/>
-      <c r="K27" s="4" t="n"/>
-      <c r="L27" s="4" t="n"/>
-      <c r="M27" s="4" t="n"/>
-      <c r="N27" s="4" t="n"/>
-      <c r="O27" s="4" t="n"/>
-      <c r="P27" s="4" t="n"/>
-      <c r="Q27" s="4" t="n"/>
-      <c r="R27" s="4" t="n"/>
-      <c r="S27" s="4" t="n"/>
-      <c r="T27" s="4" t="n"/>
-      <c r="U27" s="4" t="n"/>
-      <c r="V27" s="4" t="n"/>
-      <c r="W27" s="4" t="n"/>
-      <c r="X27" s="4" t="n"/>
-      <c r="Y27" s="4" t="n"/>
-      <c r="Z27" s="4" t="n"/>
-      <c r="AA27" s="4" t="n"/>
-      <c r="AB27" s="4" t="n"/>
-      <c r="AC27" s="4" t="n"/>
-      <c r="AD27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="n"/>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="4" t="n"/>
-      <c r="G28" s="4" t="n"/>
-      <c r="H28" s="4" t="n"/>
-      <c r="I28" s="4" t="n"/>
-      <c r="J28" s="4" t="n"/>
-      <c r="K28" s="4" t="n"/>
-      <c r="L28" s="4" t="n"/>
-      <c r="M28" s="4" t="n"/>
-      <c r="N28" s="4" t="n"/>
-      <c r="O28" s="4" t="n"/>
-      <c r="P28" s="4" t="n"/>
-      <c r="Q28" s="4" t="n"/>
-      <c r="R28" s="4" t="n"/>
-      <c r="S28" s="4" t="n"/>
-      <c r="T28" s="4" t="n"/>
-      <c r="U28" s="4" t="n"/>
-      <c r="V28" s="4" t="n"/>
-      <c r="W28" s="4" t="n"/>
-      <c r="X28" s="4" t="n"/>
-      <c r="Y28" s="4" t="n"/>
-      <c r="Z28" s="4" t="n"/>
-      <c r="AA28" s="4" t="n"/>
-      <c r="AB28" s="4" t="n"/>
-      <c r="AC28" s="4" t="n"/>
-      <c r="AD28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="4" t="n"/>
-      <c r="E29" s="4" t="n"/>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="4" t="n"/>
-      <c r="H29" s="4" t="n"/>
-      <c r="I29" s="4" t="n"/>
-      <c r="J29" s="4" t="n"/>
-      <c r="K29" s="4" t="n"/>
-      <c r="L29" s="4" t="n"/>
-      <c r="M29" s="4" t="n"/>
-      <c r="N29" s="4" t="n"/>
-      <c r="O29" s="4" t="n"/>
-      <c r="P29" s="4" t="n"/>
-      <c r="Q29" s="4" t="n"/>
-      <c r="R29" s="4" t="n"/>
-      <c r="S29" s="4" t="n"/>
-      <c r="T29" s="4" t="n"/>
-      <c r="U29" s="4" t="n"/>
-      <c r="V29" s="4" t="n"/>
-      <c r="W29" s="4" t="n"/>
-      <c r="X29" s="4" t="n"/>
-      <c r="Y29" s="4" t="n"/>
-      <c r="Z29" s="4" t="n"/>
-      <c r="AA29" s="4" t="n"/>
-      <c r="AB29" s="4" t="n"/>
-      <c r="AC29" s="4" t="n"/>
-      <c r="AD29" s="4" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="4" t="n"/>
-      <c r="E30" s="4" t="n"/>
-      <c r="F30" s="4" t="n"/>
-      <c r="G30" s="4" t="n"/>
-      <c r="H30" s="4" t="n"/>
-      <c r="I30" s="4" t="n"/>
-      <c r="J30" s="4" t="n"/>
-      <c r="K30" s="4" t="n"/>
-      <c r="L30" s="4" t="n"/>
-      <c r="M30" s="4" t="n"/>
-      <c r="N30" s="4" t="n"/>
-      <c r="O30" s="4" t="n"/>
-      <c r="P30" s="4" t="n"/>
-      <c r="Q30" s="4" t="n"/>
-      <c r="R30" s="4" t="n"/>
-      <c r="S30" s="4" t="n"/>
-      <c r="T30" s="4" t="n"/>
-      <c r="U30" s="4" t="n"/>
-      <c r="V30" s="4" t="n"/>
-      <c r="W30" s="4" t="n"/>
-      <c r="X30" s="4" t="n"/>
-      <c r="Y30" s="4" t="n"/>
-      <c r="Z30" s="4" t="n"/>
-      <c r="AA30" s="4" t="n"/>
-      <c r="AB30" s="4" t="n"/>
-      <c r="AC30" s="4" t="n"/>
-      <c r="AD30" s="4" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="n"/>
-      <c r="B31" s="4" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="4" t="n"/>
-      <c r="E31" s="4" t="n"/>
-      <c r="F31" s="4" t="n"/>
-      <c r="G31" s="4" t="n"/>
-      <c r="H31" s="4" t="n"/>
-      <c r="I31" s="4" t="n"/>
-      <c r="J31" s="4" t="n"/>
-      <c r="K31" s="4" t="n"/>
-      <c r="L31" s="4" t="n"/>
-      <c r="M31" s="4" t="n"/>
-      <c r="N31" s="4" t="n"/>
-      <c r="O31" s="4" t="n"/>
-      <c r="P31" s="4" t="n"/>
-      <c r="Q31" s="4" t="n"/>
-      <c r="R31" s="4" t="n"/>
-      <c r="S31" s="4" t="n"/>
-      <c r="T31" s="4" t="n"/>
-      <c r="U31" s="4" t="n"/>
-      <c r="V31" s="4" t="n"/>
-      <c r="W31" s="4" t="n"/>
-      <c r="X31" s="4" t="n"/>
-      <c r="Y31" s="4" t="n"/>
-      <c r="Z31" s="4" t="n"/>
-      <c r="AA31" s="4" t="n"/>
-      <c r="AB31" s="4" t="n"/>
-      <c r="AC31" s="4" t="n"/>
-      <c r="AD31" s="4" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="n"/>
-      <c r="B32" s="4" t="n"/>
-      <c r="C32" s="4" t="n"/>
-      <c r="D32" s="4" t="n"/>
-      <c r="E32" s="4" t="n"/>
-      <c r="F32" s="4" t="n"/>
-      <c r="G32" s="4" t="n"/>
-      <c r="H32" s="4" t="n"/>
-      <c r="I32" s="4" t="n"/>
-      <c r="J32" s="4" t="n"/>
-      <c r="K32" s="4" t="n"/>
-      <c r="L32" s="4" t="n"/>
-      <c r="M32" s="4" t="n"/>
-      <c r="N32" s="4" t="n"/>
-      <c r="O32" s="4" t="n"/>
-      <c r="P32" s="4" t="n"/>
-      <c r="Q32" s="4" t="n"/>
-      <c r="R32" s="4" t="n"/>
-      <c r="S32" s="4" t="n"/>
-      <c r="T32" s="4" t="n"/>
-      <c r="U32" s="4" t="n"/>
-      <c r="V32" s="4" t="n"/>
-      <c r="W32" s="4" t="n"/>
-      <c r="X32" s="4" t="n"/>
-      <c r="Y32" s="4" t="n"/>
-      <c r="Z32" s="4" t="n"/>
-      <c r="AA32" s="4" t="n"/>
-      <c r="AB32" s="4" t="n"/>
-      <c r="AC32" s="4" t="n"/>
-      <c r="AD32" s="4" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="4" t="n"/>
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
-      <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
-      <c r="H33" s="4" t="n"/>
-      <c r="I33" s="4" t="n"/>
-      <c r="J33" s="4" t="n"/>
-      <c r="K33" s="4" t="n"/>
-      <c r="L33" s="4" t="n"/>
-      <c r="M33" s="4" t="n"/>
-      <c r="N33" s="4" t="n"/>
-      <c r="O33" s="4" t="n"/>
-      <c r="P33" s="4" t="n"/>
-      <c r="Q33" s="4" t="n"/>
-      <c r="R33" s="4" t="n"/>
-      <c r="S33" s="4" t="n"/>
-      <c r="T33" s="4" t="n"/>
-      <c r="U33" s="4" t="n"/>
-      <c r="V33" s="4" t="n"/>
-      <c r="W33" s="4" t="n"/>
-      <c r="X33" s="4" t="n"/>
-      <c r="Y33" s="4" t="n"/>
-      <c r="Z33" s="4" t="n"/>
-      <c r="AA33" s="4" t="n"/>
-      <c r="AB33" s="4" t="n"/>
-      <c r="AC33" s="4" t="n"/>
-      <c r="AD33" s="4" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="n"/>
-      <c r="B34" s="4" t="n"/>
-      <c r="C34" s="4" t="n"/>
-      <c r="D34" s="4" t="n"/>
-      <c r="E34" s="4" t="n"/>
-      <c r="F34" s="4" t="n"/>
-      <c r="G34" s="4" t="n"/>
-      <c r="H34" s="4" t="n"/>
-      <c r="I34" s="4" t="n"/>
-      <c r="J34" s="4" t="n"/>
-      <c r="K34" s="4" t="n"/>
-      <c r="L34" s="4" t="n"/>
-      <c r="M34" s="4" t="n"/>
-      <c r="N34" s="4" t="n"/>
-      <c r="O34" s="4" t="n"/>
-      <c r="P34" s="4" t="n"/>
-      <c r="Q34" s="4" t="n"/>
-      <c r="R34" s="4" t="n"/>
-      <c r="S34" s="4" t="n"/>
-      <c r="T34" s="4" t="n"/>
-      <c r="U34" s="4" t="n"/>
-      <c r="V34" s="4" t="n"/>
-      <c r="W34" s="4" t="n"/>
-      <c r="X34" s="4" t="n"/>
-      <c r="Y34" s="4" t="n"/>
-      <c r="Z34" s="4" t="n"/>
-      <c r="AA34" s="4" t="n"/>
-      <c r="AB34" s="4" t="n"/>
-      <c r="AC34" s="4" t="n"/>
-      <c r="AD34" s="4" t="n"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AD36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>embeddings</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr"/>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr"/>
-      <c r="D2" s="6" t="n"/>
-      <c r="E2" s="6" t="n"/>
-      <c r="F2" s="6" t="n"/>
-      <c r="G2" s="6" t="n"/>
-      <c r="H2" s="6" t="n"/>
-      <c r="I2" s="6" t="n"/>
-      <c r="J2" s="6" t="n"/>
-      <c r="K2" s="6" t="n"/>
-      <c r="L2" s="6" t="n"/>
-      <c r="M2" s="6" t="n"/>
-      <c r="N2" s="6" t="n"/>
-      <c r="O2" s="6" t="n"/>
-      <c r="P2" s="6" t="n"/>
-      <c r="Q2" s="6" t="n"/>
-      <c r="R2" s="6" t="n"/>
-      <c r="S2" s="6" t="n"/>
-      <c r="T2" s="6" t="n"/>
-      <c r="U2" s="6" t="n"/>
-      <c r="V2" s="6" t="n"/>
-      <c r="W2" s="6" t="n"/>
-      <c r="X2" s="6" t="n"/>
-      <c r="Y2" s="6" t="n"/>
-      <c r="Z2" s="6" t="n"/>
-      <c r="AA2" s="6" t="n"/>
-      <c r="AB2" s="6" t="n"/>
-      <c r="AC2" s="6" t="n"/>
-      <c r="AD2" s="6" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr"/>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="n"/>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="n"/>
-      <c r="G3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="6" t="n"/>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="6" t="n"/>
-      <c r="L3" s="6" t="n"/>
-      <c r="M3" s="6" t="n"/>
-      <c r="N3" s="6" t="n"/>
-      <c r="O3" s="6" t="n"/>
-      <c r="P3" s="6" t="n"/>
-      <c r="Q3" s="6" t="n"/>
-      <c r="R3" s="6" t="n"/>
-      <c r="S3" s="6" t="n"/>
-      <c r="T3" s="6" t="n"/>
-      <c r="U3" s="6" t="n"/>
-      <c r="V3" s="6" t="n"/>
-      <c r="W3" s="6" t="n"/>
-      <c r="X3" s="6" t="n"/>
-      <c r="Y3" s="6" t="n"/>
-      <c r="Z3" s="6" t="n"/>
-      <c r="AA3" s="6" t="n"/>
-      <c r="AB3" s="6" t="n"/>
-      <c r="AC3" s="6" t="n"/>
-      <c r="AD3" s="6" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr"/>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="n"/>
-      <c r="D4" s="6" t="n"/>
-      <c r="E4" s="6" t="n"/>
-      <c r="F4" s="6" t="n"/>
-      <c r="G4" s="6" t="n"/>
-      <c r="H4" s="6" t="n"/>
-      <c r="I4" s="6" t="n"/>
-      <c r="J4" s="6" t="n"/>
-      <c r="K4" s="6" t="n"/>
-      <c r="L4" s="6" t="n"/>
-      <c r="M4" s="6" t="n"/>
-      <c r="N4" s="6" t="n"/>
-      <c r="O4" s="6" t="n"/>
-      <c r="P4" s="6" t="n"/>
-      <c r="Q4" s="6" t="n"/>
-      <c r="R4" s="6" t="n"/>
-      <c r="S4" s="6" t="n"/>
-      <c r="T4" s="6" t="n"/>
-      <c r="U4" s="6" t="n"/>
-      <c r="V4" s="6" t="n"/>
-      <c r="W4" s="6" t="n"/>
-      <c r="X4" s="6" t="n"/>
-      <c r="Y4" s="6" t="n"/>
-      <c r="Z4" s="6" t="n"/>
-      <c r="AA4" s="6" t="n"/>
-      <c r="AB4" s="6" t="n"/>
-      <c r="AC4" s="6" t="n"/>
-      <c r="AD4" s="6" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr"/>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>vector</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>[""]</t>
-        </is>
-      </c>
-      <c r="D5" s="6" t="n"/>
-      <c r="E5" s="6" t="n"/>
-      <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" s="6" t="n"/>
-      <c r="I5" s="6" t="n"/>
-      <c r="J5" s="6" t="n"/>
-      <c r="K5" s="6" t="n"/>
-      <c r="L5" s="6" t="n"/>
-      <c r="M5" s="6" t="n"/>
-      <c r="N5" s="6" t="n"/>
-      <c r="O5" s="6" t="n"/>
-      <c r="P5" s="6" t="n"/>
-      <c r="Q5" s="6" t="n"/>
-      <c r="R5" s="6" t="n"/>
-      <c r="S5" s="6" t="n"/>
-      <c r="T5" s="6" t="n"/>
-      <c r="U5" s="6" t="n"/>
-      <c r="V5" s="6" t="n"/>
-      <c r="W5" s="6" t="n"/>
-      <c r="X5" s="6" t="n"/>
-      <c r="Y5" s="6" t="n"/>
-      <c r="Z5" s="6" t="n"/>
-      <c r="AA5" s="6" t="n"/>
-      <c r="AB5" s="6" t="n"/>
-      <c r="AC5" s="6" t="n"/>
-      <c r="AD5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="8" t="n"/>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
-      <c r="F6" s="2" t="n"/>
-      <c r="G6" s="2" t="n"/>
-      <c r="H6" s="2" t="n"/>
-      <c r="I6" s="2" t="n"/>
-      <c r="J6" s="2" t="n"/>
-      <c r="K6" s="2" t="n"/>
-      <c r="L6" s="2" t="n"/>
-      <c r="M6" s="2" t="n"/>
-      <c r="N6" s="2" t="n"/>
-      <c r="O6" s="2" t="n"/>
-      <c r="P6" s="2" t="n"/>
-      <c r="Q6" s="2" t="n"/>
-      <c r="R6" s="2" t="n"/>
-      <c r="S6" s="2" t="n"/>
-      <c r="T6" s="2" t="n"/>
-      <c r="U6" s="2" t="n"/>
-      <c r="V6" s="2" t="n"/>
-      <c r="W6" s="2" t="n"/>
-      <c r="X6" s="2" t="n"/>
-      <c r="Y6" s="2" t="n"/>
-      <c r="Z6" s="2" t="n"/>
-      <c r="AA6" s="2" t="n"/>
-      <c r="AB6" s="2" t="n"/>
-      <c r="AC6" s="2" t="n"/>
-      <c r="AD6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n"/>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="4" t="n"/>
-      <c r="E7" s="4" t="n"/>
-      <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
-      <c r="H7" s="4" t="n"/>
-      <c r="I7" s="4" t="n"/>
-      <c r="J7" s="4" t="n"/>
-      <c r="K7" s="4" t="n"/>
-      <c r="L7" s="4" t="n"/>
-      <c r="M7" s="4" t="n"/>
-      <c r="N7" s="4" t="n"/>
-      <c r="O7" s="4" t="n"/>
-      <c r="P7" s="4" t="n"/>
-      <c r="Q7" s="4" t="n"/>
-      <c r="R7" s="4" t="n"/>
-      <c r="S7" s="4" t="n"/>
-      <c r="T7" s="4" t="n"/>
-      <c r="U7" s="4" t="n"/>
-      <c r="V7" s="4" t="n"/>
-      <c r="W7" s="4" t="n"/>
-      <c r="X7" s="4" t="n"/>
-      <c r="Y7" s="4" t="n"/>
-      <c r="Z7" s="4" t="n"/>
-      <c r="AA7" s="4" t="n"/>
-      <c r="AB7" s="4" t="n"/>
-      <c r="AC7" s="4" t="n"/>
-      <c r="AD7" s="4" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="4" t="n"/>
-      <c r="E8" s="4" t="n"/>
-      <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
-      <c r="H8" s="4" t="n"/>
-      <c r="I8" s="4" t="n"/>
-      <c r="J8" s="4" t="n"/>
-      <c r="K8" s="4" t="n"/>
-      <c r="L8" s="4" t="n"/>
-      <c r="M8" s="4" t="n"/>
-      <c r="N8" s="4" t="n"/>
-      <c r="O8" s="4" t="n"/>
-      <c r="P8" s="4" t="n"/>
-      <c r="Q8" s="4" t="n"/>
-      <c r="R8" s="4" t="n"/>
-      <c r="S8" s="4" t="n"/>
-      <c r="T8" s="4" t="n"/>
-      <c r="U8" s="4" t="n"/>
-      <c r="V8" s="4" t="n"/>
-      <c r="W8" s="4" t="n"/>
-      <c r="X8" s="4" t="n"/>
-      <c r="Y8" s="4" t="n"/>
-      <c r="Z8" s="4" t="n"/>
-      <c r="AA8" s="4" t="n"/>
-      <c r="AB8" s="4" t="n"/>
-      <c r="AC8" s="4" t="n"/>
-      <c r="AD8" s="4" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n"/>
-      <c r="B9" s="4" t="n"/>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="4" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
-      <c r="H9" s="4" t="n"/>
-      <c r="I9" s="4" t="n"/>
-      <c r="J9" s="4" t="n"/>
-      <c r="K9" s="4" t="n"/>
-      <c r="L9" s="4" t="n"/>
-      <c r="M9" s="4" t="n"/>
-      <c r="N9" s="4" t="n"/>
-      <c r="O9" s="4" t="n"/>
-      <c r="P9" s="4" t="n"/>
-      <c r="Q9" s="4" t="n"/>
-      <c r="R9" s="4" t="n"/>
-      <c r="S9" s="4" t="n"/>
-      <c r="T9" s="4" t="n"/>
-      <c r="U9" s="4" t="n"/>
-      <c r="V9" s="4" t="n"/>
-      <c r="W9" s="4" t="n"/>
-      <c r="X9" s="4" t="n"/>
-      <c r="Y9" s="4" t="n"/>
-      <c r="Z9" s="4" t="n"/>
-      <c r="AA9" s="4" t="n"/>
-      <c r="AB9" s="4" t="n"/>
-      <c r="AC9" s="4" t="n"/>
-      <c r="AD9" s="4" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n"/>
-      <c r="B10" s="4" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="4" t="n"/>
-      <c r="E10" s="4" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="4" t="n"/>
-      <c r="H10" s="4" t="n"/>
-      <c r="I10" s="4" t="n"/>
-      <c r="J10" s="4" t="n"/>
-      <c r="K10" s="4" t="n"/>
-      <c r="L10" s="4" t="n"/>
-      <c r="M10" s="4" t="n"/>
-      <c r="N10" s="4" t="n"/>
-      <c r="O10" s="4" t="n"/>
-      <c r="P10" s="4" t="n"/>
-      <c r="Q10" s="4" t="n"/>
-      <c r="R10" s="4" t="n"/>
-      <c r="S10" s="4" t="n"/>
-      <c r="T10" s="4" t="n"/>
-      <c r="U10" s="4" t="n"/>
-      <c r="V10" s="4" t="n"/>
-      <c r="W10" s="4" t="n"/>
-      <c r="X10" s="4" t="n"/>
-      <c r="Y10" s="4" t="n"/>
-      <c r="Z10" s="4" t="n"/>
-      <c r="AA10" s="4" t="n"/>
-      <c r="AB10" s="4" t="n"/>
-      <c r="AC10" s="4" t="n"/>
-      <c r="AD10" s="4" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="4" t="n"/>
-      <c r="D11" s="4" t="n"/>
-      <c r="E11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="n"/>
-      <c r="H11" s="4" t="n"/>
-      <c r="I11" s="4" t="n"/>
-      <c r="J11" s="4" t="n"/>
-      <c r="K11" s="4" t="n"/>
-      <c r="L11" s="4" t="n"/>
-      <c r="M11" s="4" t="n"/>
-      <c r="N11" s="4" t="n"/>
-      <c r="O11" s="4" t="n"/>
-      <c r="P11" s="4" t="n"/>
-      <c r="Q11" s="4" t="n"/>
-      <c r="R11" s="4" t="n"/>
-      <c r="S11" s="4" t="n"/>
-      <c r="T11" s="4" t="n"/>
-      <c r="U11" s="4" t="n"/>
-      <c r="V11" s="4" t="n"/>
-      <c r="W11" s="4" t="n"/>
-      <c r="X11" s="4" t="n"/>
-      <c r="Y11" s="4" t="n"/>
-      <c r="Z11" s="4" t="n"/>
-      <c r="AA11" s="4" t="n"/>
-      <c r="AB11" s="4" t="n"/>
-      <c r="AC11" s="4" t="n"/>
-      <c r="AD11" s="4" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="4" t="n"/>
-      <c r="J12" s="4" t="n"/>
-      <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
-      <c r="N12" s="4" t="n"/>
-      <c r="O12" s="4" t="n"/>
-      <c r="P12" s="4" t="n"/>
-      <c r="Q12" s="4" t="n"/>
-      <c r="R12" s="4" t="n"/>
-      <c r="S12" s="4" t="n"/>
-      <c r="T12" s="4" t="n"/>
-      <c r="U12" s="4" t="n"/>
-      <c r="V12" s="4" t="n"/>
-      <c r="W12" s="4" t="n"/>
-      <c r="X12" s="4" t="n"/>
-      <c r="Y12" s="4" t="n"/>
-      <c r="Z12" s="4" t="n"/>
-      <c r="AA12" s="4" t="n"/>
-      <c r="AB12" s="4" t="n"/>
-      <c r="AC12" s="4" t="n"/>
-      <c r="AD12" s="4" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n"/>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" s="4" t="n"/>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
-      <c r="H13" s="4" t="n"/>
-      <c r="I13" s="4" t="n"/>
-      <c r="J13" s="4" t="n"/>
-      <c r="K13" s="4" t="n"/>
-      <c r="L13" s="4" t="n"/>
-      <c r="M13" s="4" t="n"/>
-      <c r="N13" s="4" t="n"/>
-      <c r="O13" s="4" t="n"/>
-      <c r="P13" s="4" t="n"/>
-      <c r="Q13" s="4" t="n"/>
-      <c r="R13" s="4" t="n"/>
-      <c r="S13" s="4" t="n"/>
-      <c r="T13" s="4" t="n"/>
-      <c r="U13" s="4" t="n"/>
-      <c r="V13" s="4" t="n"/>
-      <c r="W13" s="4" t="n"/>
-      <c r="X13" s="4" t="n"/>
-      <c r="Y13" s="4" t="n"/>
-      <c r="Z13" s="4" t="n"/>
-      <c r="AA13" s="4" t="n"/>
-      <c r="AB13" s="4" t="n"/>
-      <c r="AC13" s="4" t="n"/>
-      <c r="AD13" s="4" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n"/>
-      <c r="B14" s="4" t="n"/>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="4" t="n"/>
-      <c r="E14" s="4" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="4" t="n"/>
-      <c r="I14" s="4" t="n"/>
-      <c r="J14" s="4" t="n"/>
-      <c r="K14" s="4" t="n"/>
-      <c r="L14" s="4" t="n"/>
-      <c r="M14" s="4" t="n"/>
-      <c r="N14" s="4" t="n"/>
-      <c r="O14" s="4" t="n"/>
-      <c r="P14" s="4" t="n"/>
-      <c r="Q14" s="4" t="n"/>
-      <c r="R14" s="4" t="n"/>
-      <c r="S14" s="4" t="n"/>
-      <c r="T14" s="4" t="n"/>
-      <c r="U14" s="4" t="n"/>
-      <c r="V14" s="4" t="n"/>
-      <c r="W14" s="4" t="n"/>
-      <c r="X14" s="4" t="n"/>
-      <c r="Y14" s="4" t="n"/>
-      <c r="Z14" s="4" t="n"/>
-      <c r="AA14" s="4" t="n"/>
-      <c r="AB14" s="4" t="n"/>
-      <c r="AC14" s="4" t="n"/>
-      <c r="AD14" s="4" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n"/>
-      <c r="B15" s="4" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="4" t="n"/>
-      <c r="E15" s="4" t="n"/>
-      <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="n"/>
-      <c r="H15" s="4" t="n"/>
-      <c r="I15" s="4" t="n"/>
-      <c r="J15" s="4" t="n"/>
-      <c r="K15" s="4" t="n"/>
-      <c r="L15" s="4" t="n"/>
-      <c r="M15" s="4" t="n"/>
-      <c r="N15" s="4" t="n"/>
-      <c r="O15" s="4" t="n"/>
-      <c r="P15" s="4" t="n"/>
-      <c r="Q15" s="4" t="n"/>
-      <c r="R15" s="4" t="n"/>
-      <c r="S15" s="4" t="n"/>
-      <c r="T15" s="4" t="n"/>
-      <c r="U15" s="4" t="n"/>
-      <c r="V15" s="4" t="n"/>
-      <c r="W15" s="4" t="n"/>
-      <c r="X15" s="4" t="n"/>
-      <c r="Y15" s="4" t="n"/>
-      <c r="Z15" s="4" t="n"/>
-      <c r="AA15" s="4" t="n"/>
-      <c r="AB15" s="4" t="n"/>
-      <c r="AC15" s="4" t="n"/>
-      <c r="AD15" s="4" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n"/>
-      <c r="B16" s="4" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="4" t="n"/>
-      <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="n"/>
-      <c r="H16" s="4" t="n"/>
-      <c r="I16" s="4" t="n"/>
-      <c r="J16" s="4" t="n"/>
-      <c r="K16" s="4" t="n"/>
-      <c r="L16" s="4" t="n"/>
-      <c r="M16" s="4" t="n"/>
-      <c r="N16" s="4" t="n"/>
-      <c r="O16" s="4" t="n"/>
-      <c r="P16" s="4" t="n"/>
-      <c r="Q16" s="4" t="n"/>
-      <c r="R16" s="4" t="n"/>
-      <c r="S16" s="4" t="n"/>
-      <c r="T16" s="4" t="n"/>
-      <c r="U16" s="4" t="n"/>
-      <c r="V16" s="4" t="n"/>
-      <c r="W16" s="4" t="n"/>
-      <c r="X16" s="4" t="n"/>
-      <c r="Y16" s="4" t="n"/>
-      <c r="Z16" s="4" t="n"/>
-      <c r="AA16" s="4" t="n"/>
-      <c r="AB16" s="4" t="n"/>
-      <c r="AC16" s="4" t="n"/>
-      <c r="AD16" s="4" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n"/>
-      <c r="B17" s="4" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="4" t="n"/>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
-      <c r="G17" s="4" t="n"/>
-      <c r="H17" s="4" t="n"/>
-      <c r="I17" s="4" t="n"/>
-      <c r="J17" s="4" t="n"/>
-      <c r="K17" s="4" t="n"/>
-      <c r="L17" s="4" t="n"/>
-      <c r="M17" s="4" t="n"/>
-      <c r="N17" s="4" t="n"/>
-      <c r="O17" s="4" t="n"/>
-      <c r="P17" s="4" t="n"/>
-      <c r="Q17" s="4" t="n"/>
-      <c r="R17" s="4" t="n"/>
-      <c r="S17" s="4" t="n"/>
-      <c r="T17" s="4" t="n"/>
-      <c r="U17" s="4" t="n"/>
-      <c r="V17" s="4" t="n"/>
-      <c r="W17" s="4" t="n"/>
-      <c r="X17" s="4" t="n"/>
-      <c r="Y17" s="4" t="n"/>
-      <c r="Z17" s="4" t="n"/>
-      <c r="AA17" s="4" t="n"/>
-      <c r="AB17" s="4" t="n"/>
-      <c r="AC17" s="4" t="n"/>
-      <c r="AD17" s="4" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="4" t="n"/>
-      <c r="F18" s="4" t="n"/>
-      <c r="G18" s="4" t="n"/>
-      <c r="H18" s="4" t="n"/>
-      <c r="I18" s="4" t="n"/>
-      <c r="J18" s="4" t="n"/>
-      <c r="K18" s="4" t="n"/>
-      <c r="L18" s="4" t="n"/>
-      <c r="M18" s="4" t="n"/>
-      <c r="N18" s="4" t="n"/>
-      <c r="O18" s="4" t="n"/>
-      <c r="P18" s="4" t="n"/>
-      <c r="Q18" s="4" t="n"/>
-      <c r="R18" s="4" t="n"/>
-      <c r="S18" s="4" t="n"/>
-      <c r="T18" s="4" t="n"/>
-      <c r="U18" s="4" t="n"/>
-      <c r="V18" s="4" t="n"/>
-      <c r="W18" s="4" t="n"/>
-      <c r="X18" s="4" t="n"/>
-      <c r="Y18" s="4" t="n"/>
-      <c r="Z18" s="4" t="n"/>
-      <c r="AA18" s="4" t="n"/>
-      <c r="AB18" s="4" t="n"/>
-      <c r="AC18" s="4" t="n"/>
-      <c r="AD18" s="4" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="n"/>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="4" t="n"/>
-      <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="4" t="n"/>
-      <c r="I19" s="4" t="n"/>
-      <c r="J19" s="4" t="n"/>
-      <c r="K19" s="4" t="n"/>
-      <c r="L19" s="4" t="n"/>
-      <c r="M19" s="4" t="n"/>
-      <c r="N19" s="4" t="n"/>
-      <c r="O19" s="4" t="n"/>
-      <c r="P19" s="4" t="n"/>
-      <c r="Q19" s="4" t="n"/>
-      <c r="R19" s="4" t="n"/>
-      <c r="S19" s="4" t="n"/>
-      <c r="T19" s="4" t="n"/>
-      <c r="U19" s="4" t="n"/>
-      <c r="V19" s="4" t="n"/>
-      <c r="W19" s="4" t="n"/>
-      <c r="X19" s="4" t="n"/>
-      <c r="Y19" s="4" t="n"/>
-      <c r="Z19" s="4" t="n"/>
-      <c r="AA19" s="4" t="n"/>
-      <c r="AB19" s="4" t="n"/>
-      <c r="AC19" s="4" t="n"/>
-      <c r="AD19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="4" t="n"/>
-      <c r="E20" s="4" t="n"/>
-      <c r="F20" s="4" t="n"/>
-      <c r="G20" s="4" t="n"/>
-      <c r="H20" s="4" t="n"/>
-      <c r="I20" s="4" t="n"/>
-      <c r="J20" s="4" t="n"/>
-      <c r="K20" s="4" t="n"/>
-      <c r="L20" s="4" t="n"/>
-      <c r="M20" s="4" t="n"/>
-      <c r="N20" s="4" t="n"/>
-      <c r="O20" s="4" t="n"/>
-      <c r="P20" s="4" t="n"/>
-      <c r="Q20" s="4" t="n"/>
-      <c r="R20" s="4" t="n"/>
-      <c r="S20" s="4" t="n"/>
-      <c r="T20" s="4" t="n"/>
-      <c r="U20" s="4" t="n"/>
-      <c r="V20" s="4" t="n"/>
-      <c r="W20" s="4" t="n"/>
-      <c r="X20" s="4" t="n"/>
-      <c r="Y20" s="4" t="n"/>
-      <c r="Z20" s="4" t="n"/>
-      <c r="AA20" s="4" t="n"/>
-      <c r="AB20" s="4" t="n"/>
-      <c r="AC20" s="4" t="n"/>
-      <c r="AD20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="n"/>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
-      <c r="G21" s="4" t="n"/>
-      <c r="H21" s="4" t="n"/>
-      <c r="I21" s="4" t="n"/>
-      <c r="J21" s="4" t="n"/>
-      <c r="K21" s="4" t="n"/>
-      <c r="L21" s="4" t="n"/>
-      <c r="M21" s="4" t="n"/>
-      <c r="N21" s="4" t="n"/>
-      <c r="O21" s="4" t="n"/>
-      <c r="P21" s="4" t="n"/>
-      <c r="Q21" s="4" t="n"/>
-      <c r="R21" s="4" t="n"/>
-      <c r="S21" s="4" t="n"/>
-      <c r="T21" s="4" t="n"/>
-      <c r="U21" s="4" t="n"/>
-      <c r="V21" s="4" t="n"/>
-      <c r="W21" s="4" t="n"/>
-      <c r="X21" s="4" t="n"/>
-      <c r="Y21" s="4" t="n"/>
-      <c r="Z21" s="4" t="n"/>
-      <c r="AA21" s="4" t="n"/>
-      <c r="AB21" s="4" t="n"/>
-      <c r="AC21" s="4" t="n"/>
-      <c r="AD21" s="4" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="n"/>
-      <c r="B22" s="4" t="n"/>
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
-      <c r="G22" s="4" t="n"/>
-      <c r="H22" s="4" t="n"/>
-      <c r="I22" s="4" t="n"/>
-      <c r="J22" s="4" t="n"/>
-      <c r="K22" s="4" t="n"/>
-      <c r="L22" s="4" t="n"/>
-      <c r="M22" s="4" t="n"/>
-      <c r="N22" s="4" t="n"/>
-      <c r="O22" s="4" t="n"/>
-      <c r="P22" s="4" t="n"/>
-      <c r="Q22" s="4" t="n"/>
-      <c r="R22" s="4" t="n"/>
-      <c r="S22" s="4" t="n"/>
-      <c r="T22" s="4" t="n"/>
-      <c r="U22" s="4" t="n"/>
-      <c r="V22" s="4" t="n"/>
-      <c r="W22" s="4" t="n"/>
-      <c r="X22" s="4" t="n"/>
-      <c r="Y22" s="4" t="n"/>
-      <c r="Z22" s="4" t="n"/>
-      <c r="AA22" s="4" t="n"/>
-      <c r="AB22" s="4" t="n"/>
-      <c r="AC22" s="4" t="n"/>
-      <c r="AD22" s="4" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="n"/>
-      <c r="B23" s="4" t="n"/>
-      <c r="C23" s="4" t="n"/>
-      <c r="D23" s="4" t="n"/>
-      <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
-      <c r="G23" s="4" t="n"/>
-      <c r="H23" s="4" t="n"/>
-      <c r="I23" s="4" t="n"/>
-      <c r="J23" s="4" t="n"/>
-      <c r="K23" s="4" t="n"/>
-      <c r="L23" s="4" t="n"/>
-      <c r="M23" s="4" t="n"/>
-      <c r="N23" s="4" t="n"/>
-      <c r="O23" s="4" t="n"/>
-      <c r="P23" s="4" t="n"/>
-      <c r="Q23" s="4" t="n"/>
-      <c r="R23" s="4" t="n"/>
-      <c r="S23" s="4" t="n"/>
-      <c r="T23" s="4" t="n"/>
-      <c r="U23" s="4" t="n"/>
-      <c r="V23" s="4" t="n"/>
-      <c r="W23" s="4" t="n"/>
-      <c r="X23" s="4" t="n"/>
-      <c r="Y23" s="4" t="n"/>
-      <c r="Z23" s="4" t="n"/>
-      <c r="AA23" s="4" t="n"/>
-      <c r="AB23" s="4" t="n"/>
-      <c r="AC23" s="4" t="n"/>
-      <c r="AD23" s="4" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="n"/>
-      <c r="B24" s="4" t="n"/>
-      <c r="C24" s="4" t="n"/>
-      <c r="D24" s="4" t="n"/>
-      <c r="E24" s="4" t="n"/>
-      <c r="F24" s="4" t="n"/>
-      <c r="G24" s="4" t="n"/>
-      <c r="H24" s="4" t="n"/>
-      <c r="I24" s="4" t="n"/>
-      <c r="J24" s="4" t="n"/>
-      <c r="K24" s="4" t="n"/>
-      <c r="L24" s="4" t="n"/>
-      <c r="M24" s="4" t="n"/>
-      <c r="N24" s="4" t="n"/>
-      <c r="O24" s="4" t="n"/>
-      <c r="P24" s="4" t="n"/>
-      <c r="Q24" s="4" t="n"/>
-      <c r="R24" s="4" t="n"/>
-      <c r="S24" s="4" t="n"/>
-      <c r="T24" s="4" t="n"/>
-      <c r="U24" s="4" t="n"/>
-      <c r="V24" s="4" t="n"/>
-      <c r="W24" s="4" t="n"/>
-      <c r="X24" s="4" t="n"/>
-      <c r="Y24" s="4" t="n"/>
-      <c r="Z24" s="4" t="n"/>
-      <c r="AA24" s="4" t="n"/>
-      <c r="AB24" s="4" t="n"/>
-      <c r="AC24" s="4" t="n"/>
-      <c r="AD24" s="4" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="4" t="n"/>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="4" t="n"/>
-      <c r="G25" s="4" t="n"/>
-      <c r="H25" s="4" t="n"/>
-      <c r="I25" s="4" t="n"/>
-      <c r="J25" s="4" t="n"/>
-      <c r="K25" s="4" t="n"/>
-      <c r="L25" s="4" t="n"/>
-      <c r="M25" s="4" t="n"/>
-      <c r="N25" s="4" t="n"/>
-      <c r="O25" s="4" t="n"/>
-      <c r="P25" s="4" t="n"/>
-      <c r="Q25" s="4" t="n"/>
-      <c r="R25" s="4" t="n"/>
-      <c r="S25" s="4" t="n"/>
-      <c r="T25" s="4" t="n"/>
-      <c r="U25" s="4" t="n"/>
-      <c r="V25" s="4" t="n"/>
-      <c r="W25" s="4" t="n"/>
-      <c r="X25" s="4" t="n"/>
-      <c r="Y25" s="4" t="n"/>
-      <c r="Z25" s="4" t="n"/>
-      <c r="AA25" s="4" t="n"/>
-      <c r="AB25" s="4" t="n"/>
-      <c r="AC25" s="4" t="n"/>
-      <c r="AD25" s="4" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="n"/>
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="M26" s="4" t="n"/>
-      <c r="N26" s="4" t="n"/>
-      <c r="O26" s="4" t="n"/>
-      <c r="P26" s="4" t="n"/>
-      <c r="Q26" s="4" t="n"/>
-      <c r="R26" s="4" t="n"/>
-      <c r="S26" s="4" t="n"/>
-      <c r="T26" s="4" t="n"/>
-      <c r="U26" s="4" t="n"/>
-      <c r="V26" s="4" t="n"/>
-      <c r="W26" s="4" t="n"/>
-      <c r="X26" s="4" t="n"/>
-      <c r="Y26" s="4" t="n"/>
-      <c r="Z26" s="4" t="n"/>
-      <c r="AA26" s="4" t="n"/>
-      <c r="AB26" s="4" t="n"/>
-      <c r="AC26" s="4" t="n"/>
-      <c r="AD26" s="4" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="n"/>
-      <c r="B27" s="4" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="4" t="n"/>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="4" t="n"/>
-      <c r="G27" s="4" t="n"/>
-      <c r="H27" s="4" t="n"/>
-      <c r="I27" s="4" t="n"/>
-      <c r="J27" s="4" t="n"/>
-      <c r="K27" s="4" t="n"/>
-      <c r="L27" s="4" t="n"/>
-      <c r="M27" s="4" t="n"/>
-      <c r="N27" s="4" t="n"/>
-      <c r="O27" s="4" t="n"/>
-      <c r="P27" s="4" t="n"/>
-      <c r="Q27" s="4" t="n"/>
-      <c r="R27" s="4" t="n"/>
-      <c r="S27" s="4" t="n"/>
-      <c r="T27" s="4" t="n"/>
-      <c r="U27" s="4" t="n"/>
-      <c r="V27" s="4" t="n"/>
-      <c r="W27" s="4" t="n"/>
-      <c r="X27" s="4" t="n"/>
-      <c r="Y27" s="4" t="n"/>
-      <c r="Z27" s="4" t="n"/>
-      <c r="AA27" s="4" t="n"/>
-      <c r="AB27" s="4" t="n"/>
-      <c r="AC27" s="4" t="n"/>
-      <c r="AD27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="n"/>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="4" t="n"/>
-      <c r="G28" s="4" t="n"/>
-      <c r="H28" s="4" t="n"/>
-      <c r="I28" s="4" t="n"/>
-      <c r="J28" s="4" t="n"/>
-      <c r="K28" s="4" t="n"/>
-      <c r="L28" s="4" t="n"/>
-      <c r="M28" s="4" t="n"/>
-      <c r="N28" s="4" t="n"/>
-      <c r="O28" s="4" t="n"/>
-      <c r="P28" s="4" t="n"/>
-      <c r="Q28" s="4" t="n"/>
-      <c r="R28" s="4" t="n"/>
-      <c r="S28" s="4" t="n"/>
-      <c r="T28" s="4" t="n"/>
-      <c r="U28" s="4" t="n"/>
-      <c r="V28" s="4" t="n"/>
-      <c r="W28" s="4" t="n"/>
-      <c r="X28" s="4" t="n"/>
-      <c r="Y28" s="4" t="n"/>
-      <c r="Z28" s="4" t="n"/>
-      <c r="AA28" s="4" t="n"/>
-      <c r="AB28" s="4" t="n"/>
-      <c r="AC28" s="4" t="n"/>
-      <c r="AD28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="4" t="n"/>
-      <c r="E29" s="4" t="n"/>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="4" t="n"/>
-      <c r="H29" s="4" t="n"/>
-      <c r="I29" s="4" t="n"/>
-      <c r="J29" s="4" t="n"/>
-      <c r="K29" s="4" t="n"/>
-      <c r="L29" s="4" t="n"/>
-      <c r="M29" s="4" t="n"/>
-      <c r="N29" s="4" t="n"/>
-      <c r="O29" s="4" t="n"/>
-      <c r="P29" s="4" t="n"/>
-      <c r="Q29" s="4" t="n"/>
-      <c r="R29" s="4" t="n"/>
-      <c r="S29" s="4" t="n"/>
-      <c r="T29" s="4" t="n"/>
-      <c r="U29" s="4" t="n"/>
-      <c r="V29" s="4" t="n"/>
-      <c r="W29" s="4" t="n"/>
-      <c r="X29" s="4" t="n"/>
-      <c r="Y29" s="4" t="n"/>
-      <c r="Z29" s="4" t="n"/>
-      <c r="AA29" s="4" t="n"/>
-      <c r="AB29" s="4" t="n"/>
-      <c r="AC29" s="4" t="n"/>
-      <c r="AD29" s="4" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="4" t="n"/>
-      <c r="E30" s="4" t="n"/>
-      <c r="F30" s="4" t="n"/>
-      <c r="G30" s="4" t="n"/>
-      <c r="H30" s="4" t="n"/>
-      <c r="I30" s="4" t="n"/>
-      <c r="J30" s="4" t="n"/>
-      <c r="K30" s="4" t="n"/>
-      <c r="L30" s="4" t="n"/>
-      <c r="M30" s="4" t="n"/>
-      <c r="N30" s="4" t="n"/>
-      <c r="O30" s="4" t="n"/>
-      <c r="P30" s="4" t="n"/>
-      <c r="Q30" s="4" t="n"/>
-      <c r="R30" s="4" t="n"/>
-      <c r="S30" s="4" t="n"/>
-      <c r="T30" s="4" t="n"/>
-      <c r="U30" s="4" t="n"/>
-      <c r="V30" s="4" t="n"/>
-      <c r="W30" s="4" t="n"/>
-      <c r="X30" s="4" t="n"/>
-      <c r="Y30" s="4" t="n"/>
-      <c r="Z30" s="4" t="n"/>
-      <c r="AA30" s="4" t="n"/>
-      <c r="AB30" s="4" t="n"/>
-      <c r="AC30" s="4" t="n"/>
-      <c r="AD30" s="4" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="n"/>
-      <c r="B31" s="4" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="4" t="n"/>
-      <c r="E31" s="4" t="n"/>
-      <c r="F31" s="4" t="n"/>
-      <c r="G31" s="4" t="n"/>
-      <c r="H31" s="4" t="n"/>
-      <c r="I31" s="4" t="n"/>
-      <c r="J31" s="4" t="n"/>
-      <c r="K31" s="4" t="n"/>
-      <c r="L31" s="4" t="n"/>
-      <c r="M31" s="4" t="n"/>
-      <c r="N31" s="4" t="n"/>
-      <c r="O31" s="4" t="n"/>
-      <c r="P31" s="4" t="n"/>
-      <c r="Q31" s="4" t="n"/>
-      <c r="R31" s="4" t="n"/>
-      <c r="S31" s="4" t="n"/>
-      <c r="T31" s="4" t="n"/>
-      <c r="U31" s="4" t="n"/>
-      <c r="V31" s="4" t="n"/>
-      <c r="W31" s="4" t="n"/>
-      <c r="X31" s="4" t="n"/>
-      <c r="Y31" s="4" t="n"/>
-      <c r="Z31" s="4" t="n"/>
-      <c r="AA31" s="4" t="n"/>
-      <c r="AB31" s="4" t="n"/>
-      <c r="AC31" s="4" t="n"/>
-      <c r="AD31" s="4" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="n"/>
-      <c r="B32" s="4" t="n"/>
-      <c r="C32" s="4" t="n"/>
-      <c r="D32" s="4" t="n"/>
-      <c r="E32" s="4" t="n"/>
-      <c r="F32" s="4" t="n"/>
-      <c r="G32" s="4" t="n"/>
-      <c r="H32" s="4" t="n"/>
-      <c r="I32" s="4" t="n"/>
-      <c r="J32" s="4" t="n"/>
-      <c r="K32" s="4" t="n"/>
-      <c r="L32" s="4" t="n"/>
-      <c r="M32" s="4" t="n"/>
-      <c r="N32" s="4" t="n"/>
-      <c r="O32" s="4" t="n"/>
-      <c r="P32" s="4" t="n"/>
-      <c r="Q32" s="4" t="n"/>
-      <c r="R32" s="4" t="n"/>
-      <c r="S32" s="4" t="n"/>
-      <c r="T32" s="4" t="n"/>
-      <c r="U32" s="4" t="n"/>
-      <c r="V32" s="4" t="n"/>
-      <c r="W32" s="4" t="n"/>
-      <c r="X32" s="4" t="n"/>
-      <c r="Y32" s="4" t="n"/>
-      <c r="Z32" s="4" t="n"/>
-      <c r="AA32" s="4" t="n"/>
-      <c r="AB32" s="4" t="n"/>
-      <c r="AC32" s="4" t="n"/>
-      <c r="AD32" s="4" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="4" t="n"/>
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
-      <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
-      <c r="H33" s="4" t="n"/>
-      <c r="I33" s="4" t="n"/>
-      <c r="J33" s="4" t="n"/>
-      <c r="K33" s="4" t="n"/>
-      <c r="L33" s="4" t="n"/>
-      <c r="M33" s="4" t="n"/>
-      <c r="N33" s="4" t="n"/>
-      <c r="O33" s="4" t="n"/>
-      <c r="P33" s="4" t="n"/>
-      <c r="Q33" s="4" t="n"/>
-      <c r="R33" s="4" t="n"/>
-      <c r="S33" s="4" t="n"/>
-      <c r="T33" s="4" t="n"/>
-      <c r="U33" s="4" t="n"/>
-      <c r="V33" s="4" t="n"/>
-      <c r="W33" s="4" t="n"/>
-      <c r="X33" s="4" t="n"/>
-      <c r="Y33" s="4" t="n"/>
-      <c r="Z33" s="4" t="n"/>
-      <c r="AA33" s="4" t="n"/>
-      <c r="AB33" s="4" t="n"/>
-      <c r="AC33" s="4" t="n"/>
-      <c r="AD33" s="4" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="n"/>
-      <c r="B34" s="4" t="n"/>
-      <c r="C34" s="4" t="n"/>
-      <c r="D34" s="4" t="n"/>
-      <c r="E34" s="4" t="n"/>
-      <c r="F34" s="4" t="n"/>
-      <c r="G34" s="4" t="n"/>
-      <c r="H34" s="4" t="n"/>
-      <c r="I34" s="4" t="n"/>
-      <c r="J34" s="4" t="n"/>
-      <c r="K34" s="4" t="n"/>
-      <c r="L34" s="4" t="n"/>
-      <c r="M34" s="4" t="n"/>
-      <c r="N34" s="4" t="n"/>
-      <c r="O34" s="4" t="n"/>
-      <c r="P34" s="4" t="n"/>
-      <c r="Q34" s="4" t="n"/>
-      <c r="R34" s="4" t="n"/>
-      <c r="S34" s="4" t="n"/>
-      <c r="T34" s="4" t="n"/>
-      <c r="U34" s="4" t="n"/>
-      <c r="V34" s="4" t="n"/>
-      <c r="W34" s="4" t="n"/>
-      <c r="X34" s="4" t="n"/>
-      <c r="Y34" s="4" t="n"/>
-      <c r="Z34" s="4" t="n"/>
-      <c r="AA34" s="4" t="n"/>
-      <c r="AB34" s="4" t="n"/>
-      <c r="AC34" s="4" t="n"/>
-      <c r="AD34" s="4" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="n"/>
-      <c r="B35" s="4" t="n"/>
-      <c r="C35" s="4" t="n"/>
-      <c r="D35" s="4" t="n"/>
-      <c r="E35" s="4" t="n"/>
-      <c r="F35" s="4" t="n"/>
-      <c r="G35" s="4" t="n"/>
-      <c r="H35" s="4" t="n"/>
-      <c r="I35" s="4" t="n"/>
-      <c r="J35" s="4" t="n"/>
-      <c r="K35" s="4" t="n"/>
-      <c r="L35" s="4" t="n"/>
-      <c r="M35" s="4" t="n"/>
-      <c r="N35" s="4" t="n"/>
-      <c r="O35" s="4" t="n"/>
-      <c r="P35" s="4" t="n"/>
-      <c r="Q35" s="4" t="n"/>
-      <c r="R35" s="4" t="n"/>
-      <c r="S35" s="4" t="n"/>
-      <c r="T35" s="4" t="n"/>
-      <c r="U35" s="4" t="n"/>
-      <c r="V35" s="4" t="n"/>
-      <c r="W35" s="4" t="n"/>
-      <c r="X35" s="4" t="n"/>
-      <c r="Y35" s="4" t="n"/>
-      <c r="Z35" s="4" t="n"/>
-      <c r="AA35" s="4" t="n"/>
-      <c r="AB35" s="4" t="n"/>
-      <c r="AC35" s="4" t="n"/>
-      <c r="AD35" s="4" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="n"/>
-      <c r="B36" s="4" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="4" t="n"/>
-      <c r="E36" s="4" t="n"/>
-      <c r="F36" s="4" t="n"/>
-      <c r="G36" s="4" t="n"/>
-      <c r="H36" s="4" t="n"/>
-      <c r="I36" s="4" t="n"/>
-      <c r="J36" s="4" t="n"/>
-      <c r="K36" s="4" t="n"/>
-      <c r="L36" s="4" t="n"/>
-      <c r="M36" s="4" t="n"/>
-      <c r="N36" s="4" t="n"/>
-      <c r="O36" s="4" t="n"/>
-      <c r="P36" s="4" t="n"/>
-      <c r="Q36" s="4" t="n"/>
-      <c r="R36" s="4" t="n"/>
-      <c r="S36" s="4" t="n"/>
-      <c r="T36" s="4" t="n"/>
-      <c r="U36" s="4" t="n"/>
-      <c r="V36" s="4" t="n"/>
-      <c r="W36" s="4" t="n"/>
-      <c r="X36" s="4" t="n"/>
-      <c r="Y36" s="4" t="n"/>
-      <c r="Z36" s="4" t="n"/>
-      <c r="AA36" s="4" t="n"/>
-      <c r="AB36" s="4" t="n"/>
-      <c r="AC36" s="4" t="n"/>
-      <c r="AD36" s="4" t="n"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
geospatial and image (#5)
* include resource

* make geospatial work

* test excel with non null values, fix lists and lists of lists handling, improve dictionary handling, make all embedding vectors lists not dicts

* fix image schema json; resolve issue of optional default values

* include excel files for geospatial and image

* remove LDA and Embeddings from schemas
</commit_message>
<xml_diff>
--- a/excel_sheets/Document_metadata.xlsx
+++ b/excel_sheets/Document_metadata.xlsx
@@ -12,8 +12,6 @@
     <sheet name="document_description" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="provenance" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="tags" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="lda_topics" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="embeddings" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4259,9 +4257,7 @@
           <t>url</t>
         </is>
       </c>
-      <c r="C32" s="6" t="n">
-        <v/>
-      </c>
+      <c r="C32" s="6" t="n"/>
       <c r="D32" s="6" t="n"/>
       <c r="E32" s="6" t="n"/>
       <c r="F32" s="6" t="n"/>
@@ -12533,2340 +12529,4 @@
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AD34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>lda_topics</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr"/>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>model_info</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>[{"source": null, "author": null, "version": null, "model_id": null, "nb_topics": null, "description": null, "corpus": null, "uri": null}]</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="n"/>
-      <c r="E2" s="6" t="n"/>
-      <c r="F2" s="6" t="n"/>
-      <c r="G2" s="6" t="n"/>
-      <c r="H2" s="6" t="n"/>
-      <c r="I2" s="6" t="n"/>
-      <c r="J2" s="6" t="n"/>
-      <c r="K2" s="6" t="n"/>
-      <c r="L2" s="6" t="n"/>
-      <c r="M2" s="6" t="n"/>
-      <c r="N2" s="6" t="n"/>
-      <c r="O2" s="6" t="n"/>
-      <c r="P2" s="6" t="n"/>
-      <c r="Q2" s="6" t="n"/>
-      <c r="R2" s="6" t="n"/>
-      <c r="S2" s="6" t="n"/>
-      <c r="T2" s="6" t="n"/>
-      <c r="U2" s="6" t="n"/>
-      <c r="V2" s="6" t="n"/>
-      <c r="W2" s="6" t="n"/>
-      <c r="X2" s="6" t="n"/>
-      <c r="Y2" s="6" t="n"/>
-      <c r="Z2" s="6" t="n"/>
-      <c r="AA2" s="6" t="n"/>
-      <c r="AB2" s="6" t="n"/>
-      <c r="AC2" s="6" t="n"/>
-      <c r="AD2" s="6" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr"/>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>topic_description</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[{"topic_id": null, "topic_score": null, "topic_label": null, "topic_words": [{"word": null, "word_weight": null}]}]</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="n"/>
-      <c r="G3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="6" t="n"/>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="6" t="n"/>
-      <c r="L3" s="6" t="n"/>
-      <c r="M3" s="6" t="n"/>
-      <c r="N3" s="6" t="n"/>
-      <c r="O3" s="6" t="n"/>
-      <c r="P3" s="6" t="n"/>
-      <c r="Q3" s="6" t="n"/>
-      <c r="R3" s="6" t="n"/>
-      <c r="S3" s="6" t="n"/>
-      <c r="T3" s="6" t="n"/>
-      <c r="U3" s="6" t="n"/>
-      <c r="V3" s="6" t="n"/>
-      <c r="W3" s="6" t="n"/>
-      <c r="X3" s="6" t="n"/>
-      <c r="Y3" s="6" t="n"/>
-      <c r="Z3" s="6" t="n"/>
-      <c r="AA3" s="6" t="n"/>
-      <c r="AB3" s="6" t="n"/>
-      <c r="AC3" s="6" t="n"/>
-      <c r="AD3" s="6" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="n"/>
-      <c r="B4" s="8" t="n"/>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
-      <c r="K4" s="2" t="n"/>
-      <c r="L4" s="2" t="n"/>
-      <c r="M4" s="2" t="n"/>
-      <c r="N4" s="2" t="n"/>
-      <c r="O4" s="2" t="n"/>
-      <c r="P4" s="2" t="n"/>
-      <c r="Q4" s="2" t="n"/>
-      <c r="R4" s="2" t="n"/>
-      <c r="S4" s="2" t="n"/>
-      <c r="T4" s="2" t="n"/>
-      <c r="U4" s="2" t="n"/>
-      <c r="V4" s="2" t="n"/>
-      <c r="W4" s="2" t="n"/>
-      <c r="X4" s="2" t="n"/>
-      <c r="Y4" s="2" t="n"/>
-      <c r="Z4" s="2" t="n"/>
-      <c r="AA4" s="2" t="n"/>
-      <c r="AB4" s="2" t="n"/>
-      <c r="AC4" s="2" t="n"/>
-      <c r="AD4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="n"/>
-      <c r="B5" s="4" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="4" t="n"/>
-      <c r="E5" s="4" t="n"/>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="4" t="n"/>
-      <c r="H5" s="4" t="n"/>
-      <c r="I5" s="4" t="n"/>
-      <c r="J5" s="4" t="n"/>
-      <c r="K5" s="4" t="n"/>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="4" t="n"/>
-      <c r="N5" s="4" t="n"/>
-      <c r="O5" s="4" t="n"/>
-      <c r="P5" s="4" t="n"/>
-      <c r="Q5" s="4" t="n"/>
-      <c r="R5" s="4" t="n"/>
-      <c r="S5" s="4" t="n"/>
-      <c r="T5" s="4" t="n"/>
-      <c r="U5" s="4" t="n"/>
-      <c r="V5" s="4" t="n"/>
-      <c r="W5" s="4" t="n"/>
-      <c r="X5" s="4" t="n"/>
-      <c r="Y5" s="4" t="n"/>
-      <c r="Z5" s="4" t="n"/>
-      <c r="AA5" s="4" t="n"/>
-      <c r="AB5" s="4" t="n"/>
-      <c r="AC5" s="4" t="n"/>
-      <c r="AD5" s="4" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="4" t="n"/>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="4" t="n"/>
-      <c r="E6" s="4" t="n"/>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="4" t="n"/>
-      <c r="H6" s="4" t="n"/>
-      <c r="I6" s="4" t="n"/>
-      <c r="J6" s="4" t="n"/>
-      <c r="K6" s="4" t="n"/>
-      <c r="L6" s="4" t="n"/>
-      <c r="M6" s="4" t="n"/>
-      <c r="N6" s="4" t="n"/>
-      <c r="O6" s="4" t="n"/>
-      <c r="P6" s="4" t="n"/>
-      <c r="Q6" s="4" t="n"/>
-      <c r="R6" s="4" t="n"/>
-      <c r="S6" s="4" t="n"/>
-      <c r="T6" s="4" t="n"/>
-      <c r="U6" s="4" t="n"/>
-      <c r="V6" s="4" t="n"/>
-      <c r="W6" s="4" t="n"/>
-      <c r="X6" s="4" t="n"/>
-      <c r="Y6" s="4" t="n"/>
-      <c r="Z6" s="4" t="n"/>
-      <c r="AA6" s="4" t="n"/>
-      <c r="AB6" s="4" t="n"/>
-      <c r="AC6" s="4" t="n"/>
-      <c r="AD6" s="4" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n"/>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="4" t="n"/>
-      <c r="E7" s="4" t="n"/>
-      <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
-      <c r="H7" s="4" t="n"/>
-      <c r="I7" s="4" t="n"/>
-      <c r="J7" s="4" t="n"/>
-      <c r="K7" s="4" t="n"/>
-      <c r="L7" s="4" t="n"/>
-      <c r="M7" s="4" t="n"/>
-      <c r="N7" s="4" t="n"/>
-      <c r="O7" s="4" t="n"/>
-      <c r="P7" s="4" t="n"/>
-      <c r="Q7" s="4" t="n"/>
-      <c r="R7" s="4" t="n"/>
-      <c r="S7" s="4" t="n"/>
-      <c r="T7" s="4" t="n"/>
-      <c r="U7" s="4" t="n"/>
-      <c r="V7" s="4" t="n"/>
-      <c r="W7" s="4" t="n"/>
-      <c r="X7" s="4" t="n"/>
-      <c r="Y7" s="4" t="n"/>
-      <c r="Z7" s="4" t="n"/>
-      <c r="AA7" s="4" t="n"/>
-      <c r="AB7" s="4" t="n"/>
-      <c r="AC7" s="4" t="n"/>
-      <c r="AD7" s="4" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="4" t="n"/>
-      <c r="E8" s="4" t="n"/>
-      <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
-      <c r="H8" s="4" t="n"/>
-      <c r="I8" s="4" t="n"/>
-      <c r="J8" s="4" t="n"/>
-      <c r="K8" s="4" t="n"/>
-      <c r="L8" s="4" t="n"/>
-      <c r="M8" s="4" t="n"/>
-      <c r="N8" s="4" t="n"/>
-      <c r="O8" s="4" t="n"/>
-      <c r="P8" s="4" t="n"/>
-      <c r="Q8" s="4" t="n"/>
-      <c r="R8" s="4" t="n"/>
-      <c r="S8" s="4" t="n"/>
-      <c r="T8" s="4" t="n"/>
-      <c r="U8" s="4" t="n"/>
-      <c r="V8" s="4" t="n"/>
-      <c r="W8" s="4" t="n"/>
-      <c r="X8" s="4" t="n"/>
-      <c r="Y8" s="4" t="n"/>
-      <c r="Z8" s="4" t="n"/>
-      <c r="AA8" s="4" t="n"/>
-      <c r="AB8" s="4" t="n"/>
-      <c r="AC8" s="4" t="n"/>
-      <c r="AD8" s="4" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n"/>
-      <c r="B9" s="4" t="n"/>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="4" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
-      <c r="H9" s="4" t="n"/>
-      <c r="I9" s="4" t="n"/>
-      <c r="J9" s="4" t="n"/>
-      <c r="K9" s="4" t="n"/>
-      <c r="L9" s="4" t="n"/>
-      <c r="M9" s="4" t="n"/>
-      <c r="N9" s="4" t="n"/>
-      <c r="O9" s="4" t="n"/>
-      <c r="P9" s="4" t="n"/>
-      <c r="Q9" s="4" t="n"/>
-      <c r="R9" s="4" t="n"/>
-      <c r="S9" s="4" t="n"/>
-      <c r="T9" s="4" t="n"/>
-      <c r="U9" s="4" t="n"/>
-      <c r="V9" s="4" t="n"/>
-      <c r="W9" s="4" t="n"/>
-      <c r="X9" s="4" t="n"/>
-      <c r="Y9" s="4" t="n"/>
-      <c r="Z9" s="4" t="n"/>
-      <c r="AA9" s="4" t="n"/>
-      <c r="AB9" s="4" t="n"/>
-      <c r="AC9" s="4" t="n"/>
-      <c r="AD9" s="4" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n"/>
-      <c r="B10" s="4" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="4" t="n"/>
-      <c r="E10" s="4" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="4" t="n"/>
-      <c r="H10" s="4" t="n"/>
-      <c r="I10" s="4" t="n"/>
-      <c r="J10" s="4" t="n"/>
-      <c r="K10" s="4" t="n"/>
-      <c r="L10" s="4" t="n"/>
-      <c r="M10" s="4" t="n"/>
-      <c r="N10" s="4" t="n"/>
-      <c r="O10" s="4" t="n"/>
-      <c r="P10" s="4" t="n"/>
-      <c r="Q10" s="4" t="n"/>
-      <c r="R10" s="4" t="n"/>
-      <c r="S10" s="4" t="n"/>
-      <c r="T10" s="4" t="n"/>
-      <c r="U10" s="4" t="n"/>
-      <c r="V10" s="4" t="n"/>
-      <c r="W10" s="4" t="n"/>
-      <c r="X10" s="4" t="n"/>
-      <c r="Y10" s="4" t="n"/>
-      <c r="Z10" s="4" t="n"/>
-      <c r="AA10" s="4" t="n"/>
-      <c r="AB10" s="4" t="n"/>
-      <c r="AC10" s="4" t="n"/>
-      <c r="AD10" s="4" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="4" t="n"/>
-      <c r="D11" s="4" t="n"/>
-      <c r="E11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="n"/>
-      <c r="H11" s="4" t="n"/>
-      <c r="I11" s="4" t="n"/>
-      <c r="J11" s="4" t="n"/>
-      <c r="K11" s="4" t="n"/>
-      <c r="L11" s="4" t="n"/>
-      <c r="M11" s="4" t="n"/>
-      <c r="N11" s="4" t="n"/>
-      <c r="O11" s="4" t="n"/>
-      <c r="P11" s="4" t="n"/>
-      <c r="Q11" s="4" t="n"/>
-      <c r="R11" s="4" t="n"/>
-      <c r="S11" s="4" t="n"/>
-      <c r="T11" s="4" t="n"/>
-      <c r="U11" s="4" t="n"/>
-      <c r="V11" s="4" t="n"/>
-      <c r="W11" s="4" t="n"/>
-      <c r="X11" s="4" t="n"/>
-      <c r="Y11" s="4" t="n"/>
-      <c r="Z11" s="4" t="n"/>
-      <c r="AA11" s="4" t="n"/>
-      <c r="AB11" s="4" t="n"/>
-      <c r="AC11" s="4" t="n"/>
-      <c r="AD11" s="4" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="4" t="n"/>
-      <c r="J12" s="4" t="n"/>
-      <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
-      <c r="N12" s="4" t="n"/>
-      <c r="O12" s="4" t="n"/>
-      <c r="P12" s="4" t="n"/>
-      <c r="Q12" s="4" t="n"/>
-      <c r="R12" s="4" t="n"/>
-      <c r="S12" s="4" t="n"/>
-      <c r="T12" s="4" t="n"/>
-      <c r="U12" s="4" t="n"/>
-      <c r="V12" s="4" t="n"/>
-      <c r="W12" s="4" t="n"/>
-      <c r="X12" s="4" t="n"/>
-      <c r="Y12" s="4" t="n"/>
-      <c r="Z12" s="4" t="n"/>
-      <c r="AA12" s="4" t="n"/>
-      <c r="AB12" s="4" t="n"/>
-      <c r="AC12" s="4" t="n"/>
-      <c r="AD12" s="4" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n"/>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" s="4" t="n"/>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
-      <c r="H13" s="4" t="n"/>
-      <c r="I13" s="4" t="n"/>
-      <c r="J13" s="4" t="n"/>
-      <c r="K13" s="4" t="n"/>
-      <c r="L13" s="4" t="n"/>
-      <c r="M13" s="4" t="n"/>
-      <c r="N13" s="4" t="n"/>
-      <c r="O13" s="4" t="n"/>
-      <c r="P13" s="4" t="n"/>
-      <c r="Q13" s="4" t="n"/>
-      <c r="R13" s="4" t="n"/>
-      <c r="S13" s="4" t="n"/>
-      <c r="T13" s="4" t="n"/>
-      <c r="U13" s="4" t="n"/>
-      <c r="V13" s="4" t="n"/>
-      <c r="W13" s="4" t="n"/>
-      <c r="X13" s="4" t="n"/>
-      <c r="Y13" s="4" t="n"/>
-      <c r="Z13" s="4" t="n"/>
-      <c r="AA13" s="4" t="n"/>
-      <c r="AB13" s="4" t="n"/>
-      <c r="AC13" s="4" t="n"/>
-      <c r="AD13" s="4" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n"/>
-      <c r="B14" s="4" t="n"/>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="4" t="n"/>
-      <c r="E14" s="4" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="4" t="n"/>
-      <c r="I14" s="4" t="n"/>
-      <c r="J14" s="4" t="n"/>
-      <c r="K14" s="4" t="n"/>
-      <c r="L14" s="4" t="n"/>
-      <c r="M14" s="4" t="n"/>
-      <c r="N14" s="4" t="n"/>
-      <c r="O14" s="4" t="n"/>
-      <c r="P14" s="4" t="n"/>
-      <c r="Q14" s="4" t="n"/>
-      <c r="R14" s="4" t="n"/>
-      <c r="S14" s="4" t="n"/>
-      <c r="T14" s="4" t="n"/>
-      <c r="U14" s="4" t="n"/>
-      <c r="V14" s="4" t="n"/>
-      <c r="W14" s="4" t="n"/>
-      <c r="X14" s="4" t="n"/>
-      <c r="Y14" s="4" t="n"/>
-      <c r="Z14" s="4" t="n"/>
-      <c r="AA14" s="4" t="n"/>
-      <c r="AB14" s="4" t="n"/>
-      <c r="AC14" s="4" t="n"/>
-      <c r="AD14" s="4" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n"/>
-      <c r="B15" s="4" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="4" t="n"/>
-      <c r="E15" s="4" t="n"/>
-      <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="n"/>
-      <c r="H15" s="4" t="n"/>
-      <c r="I15" s="4" t="n"/>
-      <c r="J15" s="4" t="n"/>
-      <c r="K15" s="4" t="n"/>
-      <c r="L15" s="4" t="n"/>
-      <c r="M15" s="4" t="n"/>
-      <c r="N15" s="4" t="n"/>
-      <c r="O15" s="4" t="n"/>
-      <c r="P15" s="4" t="n"/>
-      <c r="Q15" s="4" t="n"/>
-      <c r="R15" s="4" t="n"/>
-      <c r="S15" s="4" t="n"/>
-      <c r="T15" s="4" t="n"/>
-      <c r="U15" s="4" t="n"/>
-      <c r="V15" s="4" t="n"/>
-      <c r="W15" s="4" t="n"/>
-      <c r="X15" s="4" t="n"/>
-      <c r="Y15" s="4" t="n"/>
-      <c r="Z15" s="4" t="n"/>
-      <c r="AA15" s="4" t="n"/>
-      <c r="AB15" s="4" t="n"/>
-      <c r="AC15" s="4" t="n"/>
-      <c r="AD15" s="4" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n"/>
-      <c r="B16" s="4" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="4" t="n"/>
-      <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="n"/>
-      <c r="H16" s="4" t="n"/>
-      <c r="I16" s="4" t="n"/>
-      <c r="J16" s="4" t="n"/>
-      <c r="K16" s="4" t="n"/>
-      <c r="L16" s="4" t="n"/>
-      <c r="M16" s="4" t="n"/>
-      <c r="N16" s="4" t="n"/>
-      <c r="O16" s="4" t="n"/>
-      <c r="P16" s="4" t="n"/>
-      <c r="Q16" s="4" t="n"/>
-      <c r="R16" s="4" t="n"/>
-      <c r="S16" s="4" t="n"/>
-      <c r="T16" s="4" t="n"/>
-      <c r="U16" s="4" t="n"/>
-      <c r="V16" s="4" t="n"/>
-      <c r="W16" s="4" t="n"/>
-      <c r="X16" s="4" t="n"/>
-      <c r="Y16" s="4" t="n"/>
-      <c r="Z16" s="4" t="n"/>
-      <c r="AA16" s="4" t="n"/>
-      <c r="AB16" s="4" t="n"/>
-      <c r="AC16" s="4" t="n"/>
-      <c r="AD16" s="4" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n"/>
-      <c r="B17" s="4" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="4" t="n"/>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
-      <c r="G17" s="4" t="n"/>
-      <c r="H17" s="4" t="n"/>
-      <c r="I17" s="4" t="n"/>
-      <c r="J17" s="4" t="n"/>
-      <c r="K17" s="4" t="n"/>
-      <c r="L17" s="4" t="n"/>
-      <c r="M17" s="4" t="n"/>
-      <c r="N17" s="4" t="n"/>
-      <c r="O17" s="4" t="n"/>
-      <c r="P17" s="4" t="n"/>
-      <c r="Q17" s="4" t="n"/>
-      <c r="R17" s="4" t="n"/>
-      <c r="S17" s="4" t="n"/>
-      <c r="T17" s="4" t="n"/>
-      <c r="U17" s="4" t="n"/>
-      <c r="V17" s="4" t="n"/>
-      <c r="W17" s="4" t="n"/>
-      <c r="X17" s="4" t="n"/>
-      <c r="Y17" s="4" t="n"/>
-      <c r="Z17" s="4" t="n"/>
-      <c r="AA17" s="4" t="n"/>
-      <c r="AB17" s="4" t="n"/>
-      <c r="AC17" s="4" t="n"/>
-      <c r="AD17" s="4" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="4" t="n"/>
-      <c r="F18" s="4" t="n"/>
-      <c r="G18" s="4" t="n"/>
-      <c r="H18" s="4" t="n"/>
-      <c r="I18" s="4" t="n"/>
-      <c r="J18" s="4" t="n"/>
-      <c r="K18" s="4" t="n"/>
-      <c r="L18" s="4" t="n"/>
-      <c r="M18" s="4" t="n"/>
-      <c r="N18" s="4" t="n"/>
-      <c r="O18" s="4" t="n"/>
-      <c r="P18" s="4" t="n"/>
-      <c r="Q18" s="4" t="n"/>
-      <c r="R18" s="4" t="n"/>
-      <c r="S18" s="4" t="n"/>
-      <c r="T18" s="4" t="n"/>
-      <c r="U18" s="4" t="n"/>
-      <c r="V18" s="4" t="n"/>
-      <c r="W18" s="4" t="n"/>
-      <c r="X18" s="4" t="n"/>
-      <c r="Y18" s="4" t="n"/>
-      <c r="Z18" s="4" t="n"/>
-      <c r="AA18" s="4" t="n"/>
-      <c r="AB18" s="4" t="n"/>
-      <c r="AC18" s="4" t="n"/>
-      <c r="AD18" s="4" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="n"/>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="4" t="n"/>
-      <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="4" t="n"/>
-      <c r="I19" s="4" t="n"/>
-      <c r="J19" s="4" t="n"/>
-      <c r="K19" s="4" t="n"/>
-      <c r="L19" s="4" t="n"/>
-      <c r="M19" s="4" t="n"/>
-      <c r="N19" s="4" t="n"/>
-      <c r="O19" s="4" t="n"/>
-      <c r="P19" s="4" t="n"/>
-      <c r="Q19" s="4" t="n"/>
-      <c r="R19" s="4" t="n"/>
-      <c r="S19" s="4" t="n"/>
-      <c r="T19" s="4" t="n"/>
-      <c r="U19" s="4" t="n"/>
-      <c r="V19" s="4" t="n"/>
-      <c r="W19" s="4" t="n"/>
-      <c r="X19" s="4" t="n"/>
-      <c r="Y19" s="4" t="n"/>
-      <c r="Z19" s="4" t="n"/>
-      <c r="AA19" s="4" t="n"/>
-      <c r="AB19" s="4" t="n"/>
-      <c r="AC19" s="4" t="n"/>
-      <c r="AD19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="4" t="n"/>
-      <c r="E20" s="4" t="n"/>
-      <c r="F20" s="4" t="n"/>
-      <c r="G20" s="4" t="n"/>
-      <c r="H20" s="4" t="n"/>
-      <c r="I20" s="4" t="n"/>
-      <c r="J20" s="4" t="n"/>
-      <c r="K20" s="4" t="n"/>
-      <c r="L20" s="4" t="n"/>
-      <c r="M20" s="4" t="n"/>
-      <c r="N20" s="4" t="n"/>
-      <c r="O20" s="4" t="n"/>
-      <c r="P20" s="4" t="n"/>
-      <c r="Q20" s="4" t="n"/>
-      <c r="R20" s="4" t="n"/>
-      <c r="S20" s="4" t="n"/>
-      <c r="T20" s="4" t="n"/>
-      <c r="U20" s="4" t="n"/>
-      <c r="V20" s="4" t="n"/>
-      <c r="W20" s="4" t="n"/>
-      <c r="X20" s="4" t="n"/>
-      <c r="Y20" s="4" t="n"/>
-      <c r="Z20" s="4" t="n"/>
-      <c r="AA20" s="4" t="n"/>
-      <c r="AB20" s="4" t="n"/>
-      <c r="AC20" s="4" t="n"/>
-      <c r="AD20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="n"/>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
-      <c r="G21" s="4" t="n"/>
-      <c r="H21" s="4" t="n"/>
-      <c r="I21" s="4" t="n"/>
-      <c r="J21" s="4" t="n"/>
-      <c r="K21" s="4" t="n"/>
-      <c r="L21" s="4" t="n"/>
-      <c r="M21" s="4" t="n"/>
-      <c r="N21" s="4" t="n"/>
-      <c r="O21" s="4" t="n"/>
-      <c r="P21" s="4" t="n"/>
-      <c r="Q21" s="4" t="n"/>
-      <c r="R21" s="4" t="n"/>
-      <c r="S21" s="4" t="n"/>
-      <c r="T21" s="4" t="n"/>
-      <c r="U21" s="4" t="n"/>
-      <c r="V21" s="4" t="n"/>
-      <c r="W21" s="4" t="n"/>
-      <c r="X21" s="4" t="n"/>
-      <c r="Y21" s="4" t="n"/>
-      <c r="Z21" s="4" t="n"/>
-      <c r="AA21" s="4" t="n"/>
-      <c r="AB21" s="4" t="n"/>
-      <c r="AC21" s="4" t="n"/>
-      <c r="AD21" s="4" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="n"/>
-      <c r="B22" s="4" t="n"/>
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
-      <c r="G22" s="4" t="n"/>
-      <c r="H22" s="4" t="n"/>
-      <c r="I22" s="4" t="n"/>
-      <c r="J22" s="4" t="n"/>
-      <c r="K22" s="4" t="n"/>
-      <c r="L22" s="4" t="n"/>
-      <c r="M22" s="4" t="n"/>
-      <c r="N22" s="4" t="n"/>
-      <c r="O22" s="4" t="n"/>
-      <c r="P22" s="4" t="n"/>
-      <c r="Q22" s="4" t="n"/>
-      <c r="R22" s="4" t="n"/>
-      <c r="S22" s="4" t="n"/>
-      <c r="T22" s="4" t="n"/>
-      <c r="U22" s="4" t="n"/>
-      <c r="V22" s="4" t="n"/>
-      <c r="W22" s="4" t="n"/>
-      <c r="X22" s="4" t="n"/>
-      <c r="Y22" s="4" t="n"/>
-      <c r="Z22" s="4" t="n"/>
-      <c r="AA22" s="4" t="n"/>
-      <c r="AB22" s="4" t="n"/>
-      <c r="AC22" s="4" t="n"/>
-      <c r="AD22" s="4" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="n"/>
-      <c r="B23" s="4" t="n"/>
-      <c r="C23" s="4" t="n"/>
-      <c r="D23" s="4" t="n"/>
-      <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
-      <c r="G23" s="4" t="n"/>
-      <c r="H23" s="4" t="n"/>
-      <c r="I23" s="4" t="n"/>
-      <c r="J23" s="4" t="n"/>
-      <c r="K23" s="4" t="n"/>
-      <c r="L23" s="4" t="n"/>
-      <c r="M23" s="4" t="n"/>
-      <c r="N23" s="4" t="n"/>
-      <c r="O23" s="4" t="n"/>
-      <c r="P23" s="4" t="n"/>
-      <c r="Q23" s="4" t="n"/>
-      <c r="R23" s="4" t="n"/>
-      <c r="S23" s="4" t="n"/>
-      <c r="T23" s="4" t="n"/>
-      <c r="U23" s="4" t="n"/>
-      <c r="V23" s="4" t="n"/>
-      <c r="W23" s="4" t="n"/>
-      <c r="X23" s="4" t="n"/>
-      <c r="Y23" s="4" t="n"/>
-      <c r="Z23" s="4" t="n"/>
-      <c r="AA23" s="4" t="n"/>
-      <c r="AB23" s="4" t="n"/>
-      <c r="AC23" s="4" t="n"/>
-      <c r="AD23" s="4" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="n"/>
-      <c r="B24" s="4" t="n"/>
-      <c r="C24" s="4" t="n"/>
-      <c r="D24" s="4" t="n"/>
-      <c r="E24" s="4" t="n"/>
-      <c r="F24" s="4" t="n"/>
-      <c r="G24" s="4" t="n"/>
-      <c r="H24" s="4" t="n"/>
-      <c r="I24" s="4" t="n"/>
-      <c r="J24" s="4" t="n"/>
-      <c r="K24" s="4" t="n"/>
-      <c r="L24" s="4" t="n"/>
-      <c r="M24" s="4" t="n"/>
-      <c r="N24" s="4" t="n"/>
-      <c r="O24" s="4" t="n"/>
-      <c r="P24" s="4" t="n"/>
-      <c r="Q24" s="4" t="n"/>
-      <c r="R24" s="4" t="n"/>
-      <c r="S24" s="4" t="n"/>
-      <c r="T24" s="4" t="n"/>
-      <c r="U24" s="4" t="n"/>
-      <c r="V24" s="4" t="n"/>
-      <c r="W24" s="4" t="n"/>
-      <c r="X24" s="4" t="n"/>
-      <c r="Y24" s="4" t="n"/>
-      <c r="Z24" s="4" t="n"/>
-      <c r="AA24" s="4" t="n"/>
-      <c r="AB24" s="4" t="n"/>
-      <c r="AC24" s="4" t="n"/>
-      <c r="AD24" s="4" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="4" t="n"/>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="4" t="n"/>
-      <c r="G25" s="4" t="n"/>
-      <c r="H25" s="4" t="n"/>
-      <c r="I25" s="4" t="n"/>
-      <c r="J25" s="4" t="n"/>
-      <c r="K25" s="4" t="n"/>
-      <c r="L25" s="4" t="n"/>
-      <c r="M25" s="4" t="n"/>
-      <c r="N25" s="4" t="n"/>
-      <c r="O25" s="4" t="n"/>
-      <c r="P25" s="4" t="n"/>
-      <c r="Q25" s="4" t="n"/>
-      <c r="R25" s="4" t="n"/>
-      <c r="S25" s="4" t="n"/>
-      <c r="T25" s="4" t="n"/>
-      <c r="U25" s="4" t="n"/>
-      <c r="V25" s="4" t="n"/>
-      <c r="W25" s="4" t="n"/>
-      <c r="X25" s="4" t="n"/>
-      <c r="Y25" s="4" t="n"/>
-      <c r="Z25" s="4" t="n"/>
-      <c r="AA25" s="4" t="n"/>
-      <c r="AB25" s="4" t="n"/>
-      <c r="AC25" s="4" t="n"/>
-      <c r="AD25" s="4" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="n"/>
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="M26" s="4" t="n"/>
-      <c r="N26" s="4" t="n"/>
-      <c r="O26" s="4" t="n"/>
-      <c r="P26" s="4" t="n"/>
-      <c r="Q26" s="4" t="n"/>
-      <c r="R26" s="4" t="n"/>
-      <c r="S26" s="4" t="n"/>
-      <c r="T26" s="4" t="n"/>
-      <c r="U26" s="4" t="n"/>
-      <c r="V26" s="4" t="n"/>
-      <c r="W26" s="4" t="n"/>
-      <c r="X26" s="4" t="n"/>
-      <c r="Y26" s="4" t="n"/>
-      <c r="Z26" s="4" t="n"/>
-      <c r="AA26" s="4" t="n"/>
-      <c r="AB26" s="4" t="n"/>
-      <c r="AC26" s="4" t="n"/>
-      <c r="AD26" s="4" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="n"/>
-      <c r="B27" s="4" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="4" t="n"/>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="4" t="n"/>
-      <c r="G27" s="4" t="n"/>
-      <c r="H27" s="4" t="n"/>
-      <c r="I27" s="4" t="n"/>
-      <c r="J27" s="4" t="n"/>
-      <c r="K27" s="4" t="n"/>
-      <c r="L27" s="4" t="n"/>
-      <c r="M27" s="4" t="n"/>
-      <c r="N27" s="4" t="n"/>
-      <c r="O27" s="4" t="n"/>
-      <c r="P27" s="4" t="n"/>
-      <c r="Q27" s="4" t="n"/>
-      <c r="R27" s="4" t="n"/>
-      <c r="S27" s="4" t="n"/>
-      <c r="T27" s="4" t="n"/>
-      <c r="U27" s="4" t="n"/>
-      <c r="V27" s="4" t="n"/>
-      <c r="W27" s="4" t="n"/>
-      <c r="X27" s="4" t="n"/>
-      <c r="Y27" s="4" t="n"/>
-      <c r="Z27" s="4" t="n"/>
-      <c r="AA27" s="4" t="n"/>
-      <c r="AB27" s="4" t="n"/>
-      <c r="AC27" s="4" t="n"/>
-      <c r="AD27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="n"/>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="4" t="n"/>
-      <c r="G28" s="4" t="n"/>
-      <c r="H28" s="4" t="n"/>
-      <c r="I28" s="4" t="n"/>
-      <c r="J28" s="4" t="n"/>
-      <c r="K28" s="4" t="n"/>
-      <c r="L28" s="4" t="n"/>
-      <c r="M28" s="4" t="n"/>
-      <c r="N28" s="4" t="n"/>
-      <c r="O28" s="4" t="n"/>
-      <c r="P28" s="4" t="n"/>
-      <c r="Q28" s="4" t="n"/>
-      <c r="R28" s="4" t="n"/>
-      <c r="S28" s="4" t="n"/>
-      <c r="T28" s="4" t="n"/>
-      <c r="U28" s="4" t="n"/>
-      <c r="V28" s="4" t="n"/>
-      <c r="W28" s="4" t="n"/>
-      <c r="X28" s="4" t="n"/>
-      <c r="Y28" s="4" t="n"/>
-      <c r="Z28" s="4" t="n"/>
-      <c r="AA28" s="4" t="n"/>
-      <c r="AB28" s="4" t="n"/>
-      <c r="AC28" s="4" t="n"/>
-      <c r="AD28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="4" t="n"/>
-      <c r="E29" s="4" t="n"/>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="4" t="n"/>
-      <c r="H29" s="4" t="n"/>
-      <c r="I29" s="4" t="n"/>
-      <c r="J29" s="4" t="n"/>
-      <c r="K29" s="4" t="n"/>
-      <c r="L29" s="4" t="n"/>
-      <c r="M29" s="4" t="n"/>
-      <c r="N29" s="4" t="n"/>
-      <c r="O29" s="4" t="n"/>
-      <c r="P29" s="4" t="n"/>
-      <c r="Q29" s="4" t="n"/>
-      <c r="R29" s="4" t="n"/>
-      <c r="S29" s="4" t="n"/>
-      <c r="T29" s="4" t="n"/>
-      <c r="U29" s="4" t="n"/>
-      <c r="V29" s="4" t="n"/>
-      <c r="W29" s="4" t="n"/>
-      <c r="X29" s="4" t="n"/>
-      <c r="Y29" s="4" t="n"/>
-      <c r="Z29" s="4" t="n"/>
-      <c r="AA29" s="4" t="n"/>
-      <c r="AB29" s="4" t="n"/>
-      <c r="AC29" s="4" t="n"/>
-      <c r="AD29" s="4" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="4" t="n"/>
-      <c r="E30" s="4" t="n"/>
-      <c r="F30" s="4" t="n"/>
-      <c r="G30" s="4" t="n"/>
-      <c r="H30" s="4" t="n"/>
-      <c r="I30" s="4" t="n"/>
-      <c r="J30" s="4" t="n"/>
-      <c r="K30" s="4" t="n"/>
-      <c r="L30" s="4" t="n"/>
-      <c r="M30" s="4" t="n"/>
-      <c r="N30" s="4" t="n"/>
-      <c r="O30" s="4" t="n"/>
-      <c r="P30" s="4" t="n"/>
-      <c r="Q30" s="4" t="n"/>
-      <c r="R30" s="4" t="n"/>
-      <c r="S30" s="4" t="n"/>
-      <c r="T30" s="4" t="n"/>
-      <c r="U30" s="4" t="n"/>
-      <c r="V30" s="4" t="n"/>
-      <c r="W30" s="4" t="n"/>
-      <c r="X30" s="4" t="n"/>
-      <c r="Y30" s="4" t="n"/>
-      <c r="Z30" s="4" t="n"/>
-      <c r="AA30" s="4" t="n"/>
-      <c r="AB30" s="4" t="n"/>
-      <c r="AC30" s="4" t="n"/>
-      <c r="AD30" s="4" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="n"/>
-      <c r="B31" s="4" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="4" t="n"/>
-      <c r="E31" s="4" t="n"/>
-      <c r="F31" s="4" t="n"/>
-      <c r="G31" s="4" t="n"/>
-      <c r="H31" s="4" t="n"/>
-      <c r="I31" s="4" t="n"/>
-      <c r="J31" s="4" t="n"/>
-      <c r="K31" s="4" t="n"/>
-      <c r="L31" s="4" t="n"/>
-      <c r="M31" s="4" t="n"/>
-      <c r="N31" s="4" t="n"/>
-      <c r="O31" s="4" t="n"/>
-      <c r="P31" s="4" t="n"/>
-      <c r="Q31" s="4" t="n"/>
-      <c r="R31" s="4" t="n"/>
-      <c r="S31" s="4" t="n"/>
-      <c r="T31" s="4" t="n"/>
-      <c r="U31" s="4" t="n"/>
-      <c r="V31" s="4" t="n"/>
-      <c r="W31" s="4" t="n"/>
-      <c r="X31" s="4" t="n"/>
-      <c r="Y31" s="4" t="n"/>
-      <c r="Z31" s="4" t="n"/>
-      <c r="AA31" s="4" t="n"/>
-      <c r="AB31" s="4" t="n"/>
-      <c r="AC31" s="4" t="n"/>
-      <c r="AD31" s="4" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="n"/>
-      <c r="B32" s="4" t="n"/>
-      <c r="C32" s="4" t="n"/>
-      <c r="D32" s="4" t="n"/>
-      <c r="E32" s="4" t="n"/>
-      <c r="F32" s="4" t="n"/>
-      <c r="G32" s="4" t="n"/>
-      <c r="H32" s="4" t="n"/>
-      <c r="I32" s="4" t="n"/>
-      <c r="J32" s="4" t="n"/>
-      <c r="K32" s="4" t="n"/>
-      <c r="L32" s="4" t="n"/>
-      <c r="M32" s="4" t="n"/>
-      <c r="N32" s="4" t="n"/>
-      <c r="O32" s="4" t="n"/>
-      <c r="P32" s="4" t="n"/>
-      <c r="Q32" s="4" t="n"/>
-      <c r="R32" s="4" t="n"/>
-      <c r="S32" s="4" t="n"/>
-      <c r="T32" s="4" t="n"/>
-      <c r="U32" s="4" t="n"/>
-      <c r="V32" s="4" t="n"/>
-      <c r="W32" s="4" t="n"/>
-      <c r="X32" s="4" t="n"/>
-      <c r="Y32" s="4" t="n"/>
-      <c r="Z32" s="4" t="n"/>
-      <c r="AA32" s="4" t="n"/>
-      <c r="AB32" s="4" t="n"/>
-      <c r="AC32" s="4" t="n"/>
-      <c r="AD32" s="4" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="4" t="n"/>
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
-      <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
-      <c r="H33" s="4" t="n"/>
-      <c r="I33" s="4" t="n"/>
-      <c r="J33" s="4" t="n"/>
-      <c r="K33" s="4" t="n"/>
-      <c r="L33" s="4" t="n"/>
-      <c r="M33" s="4" t="n"/>
-      <c r="N33" s="4" t="n"/>
-      <c r="O33" s="4" t="n"/>
-      <c r="P33" s="4" t="n"/>
-      <c r="Q33" s="4" t="n"/>
-      <c r="R33" s="4" t="n"/>
-      <c r="S33" s="4" t="n"/>
-      <c r="T33" s="4" t="n"/>
-      <c r="U33" s="4" t="n"/>
-      <c r="V33" s="4" t="n"/>
-      <c r="W33" s="4" t="n"/>
-      <c r="X33" s="4" t="n"/>
-      <c r="Y33" s="4" t="n"/>
-      <c r="Z33" s="4" t="n"/>
-      <c r="AA33" s="4" t="n"/>
-      <c r="AB33" s="4" t="n"/>
-      <c r="AC33" s="4" t="n"/>
-      <c r="AD33" s="4" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="n"/>
-      <c r="B34" s="4" t="n"/>
-      <c r="C34" s="4" t="n"/>
-      <c r="D34" s="4" t="n"/>
-      <c r="E34" s="4" t="n"/>
-      <c r="F34" s="4" t="n"/>
-      <c r="G34" s="4" t="n"/>
-      <c r="H34" s="4" t="n"/>
-      <c r="I34" s="4" t="n"/>
-      <c r="J34" s="4" t="n"/>
-      <c r="K34" s="4" t="n"/>
-      <c r="L34" s="4" t="n"/>
-      <c r="M34" s="4" t="n"/>
-      <c r="N34" s="4" t="n"/>
-      <c r="O34" s="4" t="n"/>
-      <c r="P34" s="4" t="n"/>
-      <c r="Q34" s="4" t="n"/>
-      <c r="R34" s="4" t="n"/>
-      <c r="S34" s="4" t="n"/>
-      <c r="T34" s="4" t="n"/>
-      <c r="U34" s="4" t="n"/>
-      <c r="V34" s="4" t="n"/>
-      <c r="W34" s="4" t="n"/>
-      <c r="X34" s="4" t="n"/>
-      <c r="Y34" s="4" t="n"/>
-      <c r="Z34" s="4" t="n"/>
-      <c r="AA34" s="4" t="n"/>
-      <c r="AB34" s="4" t="n"/>
-      <c r="AC34" s="4" t="n"/>
-      <c r="AD34" s="4" t="n"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AD36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>embeddings</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
-      <c r="AA1" s="2" t="n"/>
-      <c r="AB1" s="2" t="n"/>
-      <c r="AC1" s="2" t="n"/>
-      <c r="AD1" s="2" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr"/>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v/>
-      </c>
-      <c r="D2" s="6" t="inlineStr"/>
-      <c r="E2" s="6" t="n"/>
-      <c r="F2" s="6" t="n"/>
-      <c r="G2" s="6" t="n"/>
-      <c r="H2" s="6" t="n"/>
-      <c r="I2" s="6" t="n"/>
-      <c r="J2" s="6" t="n"/>
-      <c r="K2" s="6" t="n"/>
-      <c r="L2" s="6" t="n"/>
-      <c r="M2" s="6" t="n"/>
-      <c r="N2" s="6" t="n"/>
-      <c r="O2" s="6" t="n"/>
-      <c r="P2" s="6" t="n"/>
-      <c r="Q2" s="6" t="n"/>
-      <c r="R2" s="6" t="n"/>
-      <c r="S2" s="6" t="n"/>
-      <c r="T2" s="6" t="n"/>
-      <c r="U2" s="6" t="n"/>
-      <c r="V2" s="6" t="n"/>
-      <c r="W2" s="6" t="n"/>
-      <c r="X2" s="6" t="n"/>
-      <c r="Y2" s="6" t="n"/>
-      <c r="Z2" s="6" t="n"/>
-      <c r="AA2" s="6" t="n"/>
-      <c r="AB2" s="6" t="n"/>
-      <c r="AC2" s="6" t="n"/>
-      <c r="AD2" s="6" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr"/>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v/>
-      </c>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="n"/>
-      <c r="G3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="6" t="n"/>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="6" t="n"/>
-      <c r="L3" s="6" t="n"/>
-      <c r="M3" s="6" t="n"/>
-      <c r="N3" s="6" t="n"/>
-      <c r="O3" s="6" t="n"/>
-      <c r="P3" s="6" t="n"/>
-      <c r="Q3" s="6" t="n"/>
-      <c r="R3" s="6" t="n"/>
-      <c r="S3" s="6" t="n"/>
-      <c r="T3" s="6" t="n"/>
-      <c r="U3" s="6" t="n"/>
-      <c r="V3" s="6" t="n"/>
-      <c r="W3" s="6" t="n"/>
-      <c r="X3" s="6" t="n"/>
-      <c r="Y3" s="6" t="n"/>
-      <c r="Z3" s="6" t="n"/>
-      <c r="AA3" s="6" t="n"/>
-      <c r="AB3" s="6" t="n"/>
-      <c r="AC3" s="6" t="n"/>
-      <c r="AD3" s="6" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr"/>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v/>
-      </c>
-      <c r="D4" s="6" t="n"/>
-      <c r="E4" s="6" t="n"/>
-      <c r="F4" s="6" t="n"/>
-      <c r="G4" s="6" t="n"/>
-      <c r="H4" s="6" t="n"/>
-      <c r="I4" s="6" t="n"/>
-      <c r="J4" s="6" t="n"/>
-      <c r="K4" s="6" t="n"/>
-      <c r="L4" s="6" t="n"/>
-      <c r="M4" s="6" t="n"/>
-      <c r="N4" s="6" t="n"/>
-      <c r="O4" s="6" t="n"/>
-      <c r="P4" s="6" t="n"/>
-      <c r="Q4" s="6" t="n"/>
-      <c r="R4" s="6" t="n"/>
-      <c r="S4" s="6" t="n"/>
-      <c r="T4" s="6" t="n"/>
-      <c r="U4" s="6" t="n"/>
-      <c r="V4" s="6" t="n"/>
-      <c r="W4" s="6" t="n"/>
-      <c r="X4" s="6" t="n"/>
-      <c r="Y4" s="6" t="n"/>
-      <c r="Z4" s="6" t="n"/>
-      <c r="AA4" s="6" t="n"/>
-      <c r="AB4" s="6" t="n"/>
-      <c r="AC4" s="6" t="n"/>
-      <c r="AD4" s="6" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr"/>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>vector</t>
-        </is>
-      </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="inlineStr"/>
-      <c r="E5" s="6" t="n"/>
-      <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" s="6" t="n"/>
-      <c r="I5" s="6" t="n"/>
-      <c r="J5" s="6" t="n"/>
-      <c r="K5" s="6" t="n"/>
-      <c r="L5" s="6" t="n"/>
-      <c r="M5" s="6" t="n"/>
-      <c r="N5" s="6" t="n"/>
-      <c r="O5" s="6" t="n"/>
-      <c r="P5" s="6" t="n"/>
-      <c r="Q5" s="6" t="n"/>
-      <c r="R5" s="6" t="n"/>
-      <c r="S5" s="6" t="n"/>
-      <c r="T5" s="6" t="n"/>
-      <c r="U5" s="6" t="n"/>
-      <c r="V5" s="6" t="n"/>
-      <c r="W5" s="6" t="n"/>
-      <c r="X5" s="6" t="n"/>
-      <c r="Y5" s="6" t="n"/>
-      <c r="Z5" s="6" t="n"/>
-      <c r="AA5" s="6" t="n"/>
-      <c r="AB5" s="6" t="n"/>
-      <c r="AC5" s="6" t="n"/>
-      <c r="AD5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="8" t="n"/>
-      <c r="C6" s="8" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
-      <c r="F6" s="2" t="n"/>
-      <c r="G6" s="2" t="n"/>
-      <c r="H6" s="2" t="n"/>
-      <c r="I6" s="2" t="n"/>
-      <c r="J6" s="2" t="n"/>
-      <c r="K6" s="2" t="n"/>
-      <c r="L6" s="2" t="n"/>
-      <c r="M6" s="2" t="n"/>
-      <c r="N6" s="2" t="n"/>
-      <c r="O6" s="2" t="n"/>
-      <c r="P6" s="2" t="n"/>
-      <c r="Q6" s="2" t="n"/>
-      <c r="R6" s="2" t="n"/>
-      <c r="S6" s="2" t="n"/>
-      <c r="T6" s="2" t="n"/>
-      <c r="U6" s="2" t="n"/>
-      <c r="V6" s="2" t="n"/>
-      <c r="W6" s="2" t="n"/>
-      <c r="X6" s="2" t="n"/>
-      <c r="Y6" s="2" t="n"/>
-      <c r="Z6" s="2" t="n"/>
-      <c r="AA6" s="2" t="n"/>
-      <c r="AB6" s="2" t="n"/>
-      <c r="AC6" s="2" t="n"/>
-      <c r="AD6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n"/>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="4" t="n"/>
-      <c r="E7" s="4" t="n"/>
-      <c r="F7" s="4" t="n"/>
-      <c r="G7" s="4" t="n"/>
-      <c r="H7" s="4" t="n"/>
-      <c r="I7" s="4" t="n"/>
-      <c r="J7" s="4" t="n"/>
-      <c r="K7" s="4" t="n"/>
-      <c r="L7" s="4" t="n"/>
-      <c r="M7" s="4" t="n"/>
-      <c r="N7" s="4" t="n"/>
-      <c r="O7" s="4" t="n"/>
-      <c r="P7" s="4" t="n"/>
-      <c r="Q7" s="4" t="n"/>
-      <c r="R7" s="4" t="n"/>
-      <c r="S7" s="4" t="n"/>
-      <c r="T7" s="4" t="n"/>
-      <c r="U7" s="4" t="n"/>
-      <c r="V7" s="4" t="n"/>
-      <c r="W7" s="4" t="n"/>
-      <c r="X7" s="4" t="n"/>
-      <c r="Y7" s="4" t="n"/>
-      <c r="Z7" s="4" t="n"/>
-      <c r="AA7" s="4" t="n"/>
-      <c r="AB7" s="4" t="n"/>
-      <c r="AC7" s="4" t="n"/>
-      <c r="AD7" s="4" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="4" t="n"/>
-      <c r="E8" s="4" t="n"/>
-      <c r="F8" s="4" t="n"/>
-      <c r="G8" s="4" t="n"/>
-      <c r="H8" s="4" t="n"/>
-      <c r="I8" s="4" t="n"/>
-      <c r="J8" s="4" t="n"/>
-      <c r="K8" s="4" t="n"/>
-      <c r="L8" s="4" t="n"/>
-      <c r="M8" s="4" t="n"/>
-      <c r="N8" s="4" t="n"/>
-      <c r="O8" s="4" t="n"/>
-      <c r="P8" s="4" t="n"/>
-      <c r="Q8" s="4" t="n"/>
-      <c r="R8" s="4" t="n"/>
-      <c r="S8" s="4" t="n"/>
-      <c r="T8" s="4" t="n"/>
-      <c r="U8" s="4" t="n"/>
-      <c r="V8" s="4" t="n"/>
-      <c r="W8" s="4" t="n"/>
-      <c r="X8" s="4" t="n"/>
-      <c r="Y8" s="4" t="n"/>
-      <c r="Z8" s="4" t="n"/>
-      <c r="AA8" s="4" t="n"/>
-      <c r="AB8" s="4" t="n"/>
-      <c r="AC8" s="4" t="n"/>
-      <c r="AD8" s="4" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n"/>
-      <c r="B9" s="4" t="n"/>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="4" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="n"/>
-      <c r="H9" s="4" t="n"/>
-      <c r="I9" s="4" t="n"/>
-      <c r="J9" s="4" t="n"/>
-      <c r="K9" s="4" t="n"/>
-      <c r="L9" s="4" t="n"/>
-      <c r="M9" s="4" t="n"/>
-      <c r="N9" s="4" t="n"/>
-      <c r="O9" s="4" t="n"/>
-      <c r="P9" s="4" t="n"/>
-      <c r="Q9" s="4" t="n"/>
-      <c r="R9" s="4" t="n"/>
-      <c r="S9" s="4" t="n"/>
-      <c r="T9" s="4" t="n"/>
-      <c r="U9" s="4" t="n"/>
-      <c r="V9" s="4" t="n"/>
-      <c r="W9" s="4" t="n"/>
-      <c r="X9" s="4" t="n"/>
-      <c r="Y9" s="4" t="n"/>
-      <c r="Z9" s="4" t="n"/>
-      <c r="AA9" s="4" t="n"/>
-      <c r="AB9" s="4" t="n"/>
-      <c r="AC9" s="4" t="n"/>
-      <c r="AD9" s="4" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n"/>
-      <c r="B10" s="4" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="4" t="n"/>
-      <c r="E10" s="4" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="4" t="n"/>
-      <c r="H10" s="4" t="n"/>
-      <c r="I10" s="4" t="n"/>
-      <c r="J10" s="4" t="n"/>
-      <c r="K10" s="4" t="n"/>
-      <c r="L10" s="4" t="n"/>
-      <c r="M10" s="4" t="n"/>
-      <c r="N10" s="4" t="n"/>
-      <c r="O10" s="4" t="n"/>
-      <c r="P10" s="4" t="n"/>
-      <c r="Q10" s="4" t="n"/>
-      <c r="R10" s="4" t="n"/>
-      <c r="S10" s="4" t="n"/>
-      <c r="T10" s="4" t="n"/>
-      <c r="U10" s="4" t="n"/>
-      <c r="V10" s="4" t="n"/>
-      <c r="W10" s="4" t="n"/>
-      <c r="X10" s="4" t="n"/>
-      <c r="Y10" s="4" t="n"/>
-      <c r="Z10" s="4" t="n"/>
-      <c r="AA10" s="4" t="n"/>
-      <c r="AB10" s="4" t="n"/>
-      <c r="AC10" s="4" t="n"/>
-      <c r="AD10" s="4" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n"/>
-      <c r="B11" s="4" t="n"/>
-      <c r="C11" s="4" t="n"/>
-      <c r="D11" s="4" t="n"/>
-      <c r="E11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="n"/>
-      <c r="H11" s="4" t="n"/>
-      <c r="I11" s="4" t="n"/>
-      <c r="J11" s="4" t="n"/>
-      <c r="K11" s="4" t="n"/>
-      <c r="L11" s="4" t="n"/>
-      <c r="M11" s="4" t="n"/>
-      <c r="N11" s="4" t="n"/>
-      <c r="O11" s="4" t="n"/>
-      <c r="P11" s="4" t="n"/>
-      <c r="Q11" s="4" t="n"/>
-      <c r="R11" s="4" t="n"/>
-      <c r="S11" s="4" t="n"/>
-      <c r="T11" s="4" t="n"/>
-      <c r="U11" s="4" t="n"/>
-      <c r="V11" s="4" t="n"/>
-      <c r="W11" s="4" t="n"/>
-      <c r="X11" s="4" t="n"/>
-      <c r="Y11" s="4" t="n"/>
-      <c r="Z11" s="4" t="n"/>
-      <c r="AA11" s="4" t="n"/>
-      <c r="AB11" s="4" t="n"/>
-      <c r="AC11" s="4" t="n"/>
-      <c r="AD11" s="4" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="4" t="n"/>
-      <c r="J12" s="4" t="n"/>
-      <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
-      <c r="N12" s="4" t="n"/>
-      <c r="O12" s="4" t="n"/>
-      <c r="P12" s="4" t="n"/>
-      <c r="Q12" s="4" t="n"/>
-      <c r="R12" s="4" t="n"/>
-      <c r="S12" s="4" t="n"/>
-      <c r="T12" s="4" t="n"/>
-      <c r="U12" s="4" t="n"/>
-      <c r="V12" s="4" t="n"/>
-      <c r="W12" s="4" t="n"/>
-      <c r="X12" s="4" t="n"/>
-      <c r="Y12" s="4" t="n"/>
-      <c r="Z12" s="4" t="n"/>
-      <c r="AA12" s="4" t="n"/>
-      <c r="AB12" s="4" t="n"/>
-      <c r="AC12" s="4" t="n"/>
-      <c r="AD12" s="4" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n"/>
-      <c r="B13" s="4" t="n"/>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" s="4" t="n"/>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
-      <c r="H13" s="4" t="n"/>
-      <c r="I13" s="4" t="n"/>
-      <c r="J13" s="4" t="n"/>
-      <c r="K13" s="4" t="n"/>
-      <c r="L13" s="4" t="n"/>
-      <c r="M13" s="4" t="n"/>
-      <c r="N13" s="4" t="n"/>
-      <c r="O13" s="4" t="n"/>
-      <c r="P13" s="4" t="n"/>
-      <c r="Q13" s="4" t="n"/>
-      <c r="R13" s="4" t="n"/>
-      <c r="S13" s="4" t="n"/>
-      <c r="T13" s="4" t="n"/>
-      <c r="U13" s="4" t="n"/>
-      <c r="V13" s="4" t="n"/>
-      <c r="W13" s="4" t="n"/>
-      <c r="X13" s="4" t="n"/>
-      <c r="Y13" s="4" t="n"/>
-      <c r="Z13" s="4" t="n"/>
-      <c r="AA13" s="4" t="n"/>
-      <c r="AB13" s="4" t="n"/>
-      <c r="AC13" s="4" t="n"/>
-      <c r="AD13" s="4" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n"/>
-      <c r="B14" s="4" t="n"/>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="4" t="n"/>
-      <c r="E14" s="4" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="4" t="n"/>
-      <c r="I14" s="4" t="n"/>
-      <c r="J14" s="4" t="n"/>
-      <c r="K14" s="4" t="n"/>
-      <c r="L14" s="4" t="n"/>
-      <c r="M14" s="4" t="n"/>
-      <c r="N14" s="4" t="n"/>
-      <c r="O14" s="4" t="n"/>
-      <c r="P14" s="4" t="n"/>
-      <c r="Q14" s="4" t="n"/>
-      <c r="R14" s="4" t="n"/>
-      <c r="S14" s="4" t="n"/>
-      <c r="T14" s="4" t="n"/>
-      <c r="U14" s="4" t="n"/>
-      <c r="V14" s="4" t="n"/>
-      <c r="W14" s="4" t="n"/>
-      <c r="X14" s="4" t="n"/>
-      <c r="Y14" s="4" t="n"/>
-      <c r="Z14" s="4" t="n"/>
-      <c r="AA14" s="4" t="n"/>
-      <c r="AB14" s="4" t="n"/>
-      <c r="AC14" s="4" t="n"/>
-      <c r="AD14" s="4" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n"/>
-      <c r="B15" s="4" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="4" t="n"/>
-      <c r="E15" s="4" t="n"/>
-      <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="n"/>
-      <c r="H15" s="4" t="n"/>
-      <c r="I15" s="4" t="n"/>
-      <c r="J15" s="4" t="n"/>
-      <c r="K15" s="4" t="n"/>
-      <c r="L15" s="4" t="n"/>
-      <c r="M15" s="4" t="n"/>
-      <c r="N15" s="4" t="n"/>
-      <c r="O15" s="4" t="n"/>
-      <c r="P15" s="4" t="n"/>
-      <c r="Q15" s="4" t="n"/>
-      <c r="R15" s="4" t="n"/>
-      <c r="S15" s="4" t="n"/>
-      <c r="T15" s="4" t="n"/>
-      <c r="U15" s="4" t="n"/>
-      <c r="V15" s="4" t="n"/>
-      <c r="W15" s="4" t="n"/>
-      <c r="X15" s="4" t="n"/>
-      <c r="Y15" s="4" t="n"/>
-      <c r="Z15" s="4" t="n"/>
-      <c r="AA15" s="4" t="n"/>
-      <c r="AB15" s="4" t="n"/>
-      <c r="AC15" s="4" t="n"/>
-      <c r="AD15" s="4" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n"/>
-      <c r="B16" s="4" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="4" t="n"/>
-      <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="n"/>
-      <c r="H16" s="4" t="n"/>
-      <c r="I16" s="4" t="n"/>
-      <c r="J16" s="4" t="n"/>
-      <c r="K16" s="4" t="n"/>
-      <c r="L16" s="4" t="n"/>
-      <c r="M16" s="4" t="n"/>
-      <c r="N16" s="4" t="n"/>
-      <c r="O16" s="4" t="n"/>
-      <c r="P16" s="4" t="n"/>
-      <c r="Q16" s="4" t="n"/>
-      <c r="R16" s="4" t="n"/>
-      <c r="S16" s="4" t="n"/>
-      <c r="T16" s="4" t="n"/>
-      <c r="U16" s="4" t="n"/>
-      <c r="V16" s="4" t="n"/>
-      <c r="W16" s="4" t="n"/>
-      <c r="X16" s="4" t="n"/>
-      <c r="Y16" s="4" t="n"/>
-      <c r="Z16" s="4" t="n"/>
-      <c r="AA16" s="4" t="n"/>
-      <c r="AB16" s="4" t="n"/>
-      <c r="AC16" s="4" t="n"/>
-      <c r="AD16" s="4" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n"/>
-      <c r="B17" s="4" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="4" t="n"/>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
-      <c r="G17" s="4" t="n"/>
-      <c r="H17" s="4" t="n"/>
-      <c r="I17" s="4" t="n"/>
-      <c r="J17" s="4" t="n"/>
-      <c r="K17" s="4" t="n"/>
-      <c r="L17" s="4" t="n"/>
-      <c r="M17" s="4" t="n"/>
-      <c r="N17" s="4" t="n"/>
-      <c r="O17" s="4" t="n"/>
-      <c r="P17" s="4" t="n"/>
-      <c r="Q17" s="4" t="n"/>
-      <c r="R17" s="4" t="n"/>
-      <c r="S17" s="4" t="n"/>
-      <c r="T17" s="4" t="n"/>
-      <c r="U17" s="4" t="n"/>
-      <c r="V17" s="4" t="n"/>
-      <c r="W17" s="4" t="n"/>
-      <c r="X17" s="4" t="n"/>
-      <c r="Y17" s="4" t="n"/>
-      <c r="Z17" s="4" t="n"/>
-      <c r="AA17" s="4" t="n"/>
-      <c r="AB17" s="4" t="n"/>
-      <c r="AC17" s="4" t="n"/>
-      <c r="AD17" s="4" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="4" t="n"/>
-      <c r="F18" s="4" t="n"/>
-      <c r="G18" s="4" t="n"/>
-      <c r="H18" s="4" t="n"/>
-      <c r="I18" s="4" t="n"/>
-      <c r="J18" s="4" t="n"/>
-      <c r="K18" s="4" t="n"/>
-      <c r="L18" s="4" t="n"/>
-      <c r="M18" s="4" t="n"/>
-      <c r="N18" s="4" t="n"/>
-      <c r="O18" s="4" t="n"/>
-      <c r="P18" s="4" t="n"/>
-      <c r="Q18" s="4" t="n"/>
-      <c r="R18" s="4" t="n"/>
-      <c r="S18" s="4" t="n"/>
-      <c r="T18" s="4" t="n"/>
-      <c r="U18" s="4" t="n"/>
-      <c r="V18" s="4" t="n"/>
-      <c r="W18" s="4" t="n"/>
-      <c r="X18" s="4" t="n"/>
-      <c r="Y18" s="4" t="n"/>
-      <c r="Z18" s="4" t="n"/>
-      <c r="AA18" s="4" t="n"/>
-      <c r="AB18" s="4" t="n"/>
-      <c r="AC18" s="4" t="n"/>
-      <c r="AD18" s="4" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="n"/>
-      <c r="B19" s="4" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="4" t="n"/>
-      <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="4" t="n"/>
-      <c r="I19" s="4" t="n"/>
-      <c r="J19" s="4" t="n"/>
-      <c r="K19" s="4" t="n"/>
-      <c r="L19" s="4" t="n"/>
-      <c r="M19" s="4" t="n"/>
-      <c r="N19" s="4" t="n"/>
-      <c r="O19" s="4" t="n"/>
-      <c r="P19" s="4" t="n"/>
-      <c r="Q19" s="4" t="n"/>
-      <c r="R19" s="4" t="n"/>
-      <c r="S19" s="4" t="n"/>
-      <c r="T19" s="4" t="n"/>
-      <c r="U19" s="4" t="n"/>
-      <c r="V19" s="4" t="n"/>
-      <c r="W19" s="4" t="n"/>
-      <c r="X19" s="4" t="n"/>
-      <c r="Y19" s="4" t="n"/>
-      <c r="Z19" s="4" t="n"/>
-      <c r="AA19" s="4" t="n"/>
-      <c r="AB19" s="4" t="n"/>
-      <c r="AC19" s="4" t="n"/>
-      <c r="AD19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="n"/>
-      <c r="B20" s="4" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="4" t="n"/>
-      <c r="E20" s="4" t="n"/>
-      <c r="F20" s="4" t="n"/>
-      <c r="G20" s="4" t="n"/>
-      <c r="H20" s="4" t="n"/>
-      <c r="I20" s="4" t="n"/>
-      <c r="J20" s="4" t="n"/>
-      <c r="K20" s="4" t="n"/>
-      <c r="L20" s="4" t="n"/>
-      <c r="M20" s="4" t="n"/>
-      <c r="N20" s="4" t="n"/>
-      <c r="O20" s="4" t="n"/>
-      <c r="P20" s="4" t="n"/>
-      <c r="Q20" s="4" t="n"/>
-      <c r="R20" s="4" t="n"/>
-      <c r="S20" s="4" t="n"/>
-      <c r="T20" s="4" t="n"/>
-      <c r="U20" s="4" t="n"/>
-      <c r="V20" s="4" t="n"/>
-      <c r="W20" s="4" t="n"/>
-      <c r="X20" s="4" t="n"/>
-      <c r="Y20" s="4" t="n"/>
-      <c r="Z20" s="4" t="n"/>
-      <c r="AA20" s="4" t="n"/>
-      <c r="AB20" s="4" t="n"/>
-      <c r="AC20" s="4" t="n"/>
-      <c r="AD20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="n"/>
-      <c r="B21" s="4" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
-      <c r="G21" s="4" t="n"/>
-      <c r="H21" s="4" t="n"/>
-      <c r="I21" s="4" t="n"/>
-      <c r="J21" s="4" t="n"/>
-      <c r="K21" s="4" t="n"/>
-      <c r="L21" s="4" t="n"/>
-      <c r="M21" s="4" t="n"/>
-      <c r="N21" s="4" t="n"/>
-      <c r="O21" s="4" t="n"/>
-      <c r="P21" s="4" t="n"/>
-      <c r="Q21" s="4" t="n"/>
-      <c r="R21" s="4" t="n"/>
-      <c r="S21" s="4" t="n"/>
-      <c r="T21" s="4" t="n"/>
-      <c r="U21" s="4" t="n"/>
-      <c r="V21" s="4" t="n"/>
-      <c r="W21" s="4" t="n"/>
-      <c r="X21" s="4" t="n"/>
-      <c r="Y21" s="4" t="n"/>
-      <c r="Z21" s="4" t="n"/>
-      <c r="AA21" s="4" t="n"/>
-      <c r="AB21" s="4" t="n"/>
-      <c r="AC21" s="4" t="n"/>
-      <c r="AD21" s="4" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="n"/>
-      <c r="B22" s="4" t="n"/>
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
-      <c r="G22" s="4" t="n"/>
-      <c r="H22" s="4" t="n"/>
-      <c r="I22" s="4" t="n"/>
-      <c r="J22" s="4" t="n"/>
-      <c r="K22" s="4" t="n"/>
-      <c r="L22" s="4" t="n"/>
-      <c r="M22" s="4" t="n"/>
-      <c r="N22" s="4" t="n"/>
-      <c r="O22" s="4" t="n"/>
-      <c r="P22" s="4" t="n"/>
-      <c r="Q22" s="4" t="n"/>
-      <c r="R22" s="4" t="n"/>
-      <c r="S22" s="4" t="n"/>
-      <c r="T22" s="4" t="n"/>
-      <c r="U22" s="4" t="n"/>
-      <c r="V22" s="4" t="n"/>
-      <c r="W22" s="4" t="n"/>
-      <c r="X22" s="4" t="n"/>
-      <c r="Y22" s="4" t="n"/>
-      <c r="Z22" s="4" t="n"/>
-      <c r="AA22" s="4" t="n"/>
-      <c r="AB22" s="4" t="n"/>
-      <c r="AC22" s="4" t="n"/>
-      <c r="AD22" s="4" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="n"/>
-      <c r="B23" s="4" t="n"/>
-      <c r="C23" s="4" t="n"/>
-      <c r="D23" s="4" t="n"/>
-      <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
-      <c r="G23" s="4" t="n"/>
-      <c r="H23" s="4" t="n"/>
-      <c r="I23" s="4" t="n"/>
-      <c r="J23" s="4" t="n"/>
-      <c r="K23" s="4" t="n"/>
-      <c r="L23" s="4" t="n"/>
-      <c r="M23" s="4" t="n"/>
-      <c r="N23" s="4" t="n"/>
-      <c r="O23" s="4" t="n"/>
-      <c r="P23" s="4" t="n"/>
-      <c r="Q23" s="4" t="n"/>
-      <c r="R23" s="4" t="n"/>
-      <c r="S23" s="4" t="n"/>
-      <c r="T23" s="4" t="n"/>
-      <c r="U23" s="4" t="n"/>
-      <c r="V23" s="4" t="n"/>
-      <c r="W23" s="4" t="n"/>
-      <c r="X23" s="4" t="n"/>
-      <c r="Y23" s="4" t="n"/>
-      <c r="Z23" s="4" t="n"/>
-      <c r="AA23" s="4" t="n"/>
-      <c r="AB23" s="4" t="n"/>
-      <c r="AC23" s="4" t="n"/>
-      <c r="AD23" s="4" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="n"/>
-      <c r="B24" s="4" t="n"/>
-      <c r="C24" s="4" t="n"/>
-      <c r="D24" s="4" t="n"/>
-      <c r="E24" s="4" t="n"/>
-      <c r="F24" s="4" t="n"/>
-      <c r="G24" s="4" t="n"/>
-      <c r="H24" s="4" t="n"/>
-      <c r="I24" s="4" t="n"/>
-      <c r="J24" s="4" t="n"/>
-      <c r="K24" s="4" t="n"/>
-      <c r="L24" s="4" t="n"/>
-      <c r="M24" s="4" t="n"/>
-      <c r="N24" s="4" t="n"/>
-      <c r="O24" s="4" t="n"/>
-      <c r="P24" s="4" t="n"/>
-      <c r="Q24" s="4" t="n"/>
-      <c r="R24" s="4" t="n"/>
-      <c r="S24" s="4" t="n"/>
-      <c r="T24" s="4" t="n"/>
-      <c r="U24" s="4" t="n"/>
-      <c r="V24" s="4" t="n"/>
-      <c r="W24" s="4" t="n"/>
-      <c r="X24" s="4" t="n"/>
-      <c r="Y24" s="4" t="n"/>
-      <c r="Z24" s="4" t="n"/>
-      <c r="AA24" s="4" t="n"/>
-      <c r="AB24" s="4" t="n"/>
-      <c r="AC24" s="4" t="n"/>
-      <c r="AD24" s="4" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="4" t="n"/>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="4" t="n"/>
-      <c r="G25" s="4" t="n"/>
-      <c r="H25" s="4" t="n"/>
-      <c r="I25" s="4" t="n"/>
-      <c r="J25" s="4" t="n"/>
-      <c r="K25" s="4" t="n"/>
-      <c r="L25" s="4" t="n"/>
-      <c r="M25" s="4" t="n"/>
-      <c r="N25" s="4" t="n"/>
-      <c r="O25" s="4" t="n"/>
-      <c r="P25" s="4" t="n"/>
-      <c r="Q25" s="4" t="n"/>
-      <c r="R25" s="4" t="n"/>
-      <c r="S25" s="4" t="n"/>
-      <c r="T25" s="4" t="n"/>
-      <c r="U25" s="4" t="n"/>
-      <c r="V25" s="4" t="n"/>
-      <c r="W25" s="4" t="n"/>
-      <c r="X25" s="4" t="n"/>
-      <c r="Y25" s="4" t="n"/>
-      <c r="Z25" s="4" t="n"/>
-      <c r="AA25" s="4" t="n"/>
-      <c r="AB25" s="4" t="n"/>
-      <c r="AC25" s="4" t="n"/>
-      <c r="AD25" s="4" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="n"/>
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="M26" s="4" t="n"/>
-      <c r="N26" s="4" t="n"/>
-      <c r="O26" s="4" t="n"/>
-      <c r="P26" s="4" t="n"/>
-      <c r="Q26" s="4" t="n"/>
-      <c r="R26" s="4" t="n"/>
-      <c r="S26" s="4" t="n"/>
-      <c r="T26" s="4" t="n"/>
-      <c r="U26" s="4" t="n"/>
-      <c r="V26" s="4" t="n"/>
-      <c r="W26" s="4" t="n"/>
-      <c r="X26" s="4" t="n"/>
-      <c r="Y26" s="4" t="n"/>
-      <c r="Z26" s="4" t="n"/>
-      <c r="AA26" s="4" t="n"/>
-      <c r="AB26" s="4" t="n"/>
-      <c r="AC26" s="4" t="n"/>
-      <c r="AD26" s="4" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="n"/>
-      <c r="B27" s="4" t="n"/>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="4" t="n"/>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="4" t="n"/>
-      <c r="G27" s="4" t="n"/>
-      <c r="H27" s="4" t="n"/>
-      <c r="I27" s="4" t="n"/>
-      <c r="J27" s="4" t="n"/>
-      <c r="K27" s="4" t="n"/>
-      <c r="L27" s="4" t="n"/>
-      <c r="M27" s="4" t="n"/>
-      <c r="N27" s="4" t="n"/>
-      <c r="O27" s="4" t="n"/>
-      <c r="P27" s="4" t="n"/>
-      <c r="Q27" s="4" t="n"/>
-      <c r="R27" s="4" t="n"/>
-      <c r="S27" s="4" t="n"/>
-      <c r="T27" s="4" t="n"/>
-      <c r="U27" s="4" t="n"/>
-      <c r="V27" s="4" t="n"/>
-      <c r="W27" s="4" t="n"/>
-      <c r="X27" s="4" t="n"/>
-      <c r="Y27" s="4" t="n"/>
-      <c r="Z27" s="4" t="n"/>
-      <c r="AA27" s="4" t="n"/>
-      <c r="AB27" s="4" t="n"/>
-      <c r="AC27" s="4" t="n"/>
-      <c r="AD27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="n"/>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="4" t="n"/>
-      <c r="G28" s="4" t="n"/>
-      <c r="H28" s="4" t="n"/>
-      <c r="I28" s="4" t="n"/>
-      <c r="J28" s="4" t="n"/>
-      <c r="K28" s="4" t="n"/>
-      <c r="L28" s="4" t="n"/>
-      <c r="M28" s="4" t="n"/>
-      <c r="N28" s="4" t="n"/>
-      <c r="O28" s="4" t="n"/>
-      <c r="P28" s="4" t="n"/>
-      <c r="Q28" s="4" t="n"/>
-      <c r="R28" s="4" t="n"/>
-      <c r="S28" s="4" t="n"/>
-      <c r="T28" s="4" t="n"/>
-      <c r="U28" s="4" t="n"/>
-      <c r="V28" s="4" t="n"/>
-      <c r="W28" s="4" t="n"/>
-      <c r="X28" s="4" t="n"/>
-      <c r="Y28" s="4" t="n"/>
-      <c r="Z28" s="4" t="n"/>
-      <c r="AA28" s="4" t="n"/>
-      <c r="AB28" s="4" t="n"/>
-      <c r="AC28" s="4" t="n"/>
-      <c r="AD28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="4" t="n"/>
-      <c r="E29" s="4" t="n"/>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="4" t="n"/>
-      <c r="H29" s="4" t="n"/>
-      <c r="I29" s="4" t="n"/>
-      <c r="J29" s="4" t="n"/>
-      <c r="K29" s="4" t="n"/>
-      <c r="L29" s="4" t="n"/>
-      <c r="M29" s="4" t="n"/>
-      <c r="N29" s="4" t="n"/>
-      <c r="O29" s="4" t="n"/>
-      <c r="P29" s="4" t="n"/>
-      <c r="Q29" s="4" t="n"/>
-      <c r="R29" s="4" t="n"/>
-      <c r="S29" s="4" t="n"/>
-      <c r="T29" s="4" t="n"/>
-      <c r="U29" s="4" t="n"/>
-      <c r="V29" s="4" t="n"/>
-      <c r="W29" s="4" t="n"/>
-      <c r="X29" s="4" t="n"/>
-      <c r="Y29" s="4" t="n"/>
-      <c r="Z29" s="4" t="n"/>
-      <c r="AA29" s="4" t="n"/>
-      <c r="AB29" s="4" t="n"/>
-      <c r="AC29" s="4" t="n"/>
-      <c r="AD29" s="4" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="n"/>
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="4" t="n"/>
-      <c r="E30" s="4" t="n"/>
-      <c r="F30" s="4" t="n"/>
-      <c r="G30" s="4" t="n"/>
-      <c r="H30" s="4" t="n"/>
-      <c r="I30" s="4" t="n"/>
-      <c r="J30" s="4" t="n"/>
-      <c r="K30" s="4" t="n"/>
-      <c r="L30" s="4" t="n"/>
-      <c r="M30" s="4" t="n"/>
-      <c r="N30" s="4" t="n"/>
-      <c r="O30" s="4" t="n"/>
-      <c r="P30" s="4" t="n"/>
-      <c r="Q30" s="4" t="n"/>
-      <c r="R30" s="4" t="n"/>
-      <c r="S30" s="4" t="n"/>
-      <c r="T30" s="4" t="n"/>
-      <c r="U30" s="4" t="n"/>
-      <c r="V30" s="4" t="n"/>
-      <c r="W30" s="4" t="n"/>
-      <c r="X30" s="4" t="n"/>
-      <c r="Y30" s="4" t="n"/>
-      <c r="Z30" s="4" t="n"/>
-      <c r="AA30" s="4" t="n"/>
-      <c r="AB30" s="4" t="n"/>
-      <c r="AC30" s="4" t="n"/>
-      <c r="AD30" s="4" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="n"/>
-      <c r="B31" s="4" t="n"/>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="4" t="n"/>
-      <c r="E31" s="4" t="n"/>
-      <c r="F31" s="4" t="n"/>
-      <c r="G31" s="4" t="n"/>
-      <c r="H31" s="4" t="n"/>
-      <c r="I31" s="4" t="n"/>
-      <c r="J31" s="4" t="n"/>
-      <c r="K31" s="4" t="n"/>
-      <c r="L31" s="4" t="n"/>
-      <c r="M31" s="4" t="n"/>
-      <c r="N31" s="4" t="n"/>
-      <c r="O31" s="4" t="n"/>
-      <c r="P31" s="4" t="n"/>
-      <c r="Q31" s="4" t="n"/>
-      <c r="R31" s="4" t="n"/>
-      <c r="S31" s="4" t="n"/>
-      <c r="T31" s="4" t="n"/>
-      <c r="U31" s="4" t="n"/>
-      <c r="V31" s="4" t="n"/>
-      <c r="W31" s="4" t="n"/>
-      <c r="X31" s="4" t="n"/>
-      <c r="Y31" s="4" t="n"/>
-      <c r="Z31" s="4" t="n"/>
-      <c r="AA31" s="4" t="n"/>
-      <c r="AB31" s="4" t="n"/>
-      <c r="AC31" s="4" t="n"/>
-      <c r="AD31" s="4" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="n"/>
-      <c r="B32" s="4" t="n"/>
-      <c r="C32" s="4" t="n"/>
-      <c r="D32" s="4" t="n"/>
-      <c r="E32" s="4" t="n"/>
-      <c r="F32" s="4" t="n"/>
-      <c r="G32" s="4" t="n"/>
-      <c r="H32" s="4" t="n"/>
-      <c r="I32" s="4" t="n"/>
-      <c r="J32" s="4" t="n"/>
-      <c r="K32" s="4" t="n"/>
-      <c r="L32" s="4" t="n"/>
-      <c r="M32" s="4" t="n"/>
-      <c r="N32" s="4" t="n"/>
-      <c r="O32" s="4" t="n"/>
-      <c r="P32" s="4" t="n"/>
-      <c r="Q32" s="4" t="n"/>
-      <c r="R32" s="4" t="n"/>
-      <c r="S32" s="4" t="n"/>
-      <c r="T32" s="4" t="n"/>
-      <c r="U32" s="4" t="n"/>
-      <c r="V32" s="4" t="n"/>
-      <c r="W32" s="4" t="n"/>
-      <c r="X32" s="4" t="n"/>
-      <c r="Y32" s="4" t="n"/>
-      <c r="Z32" s="4" t="n"/>
-      <c r="AA32" s="4" t="n"/>
-      <c r="AB32" s="4" t="n"/>
-      <c r="AC32" s="4" t="n"/>
-      <c r="AD32" s="4" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="4" t="n"/>
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
-      <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
-      <c r="H33" s="4" t="n"/>
-      <c r="I33" s="4" t="n"/>
-      <c r="J33" s="4" t="n"/>
-      <c r="K33" s="4" t="n"/>
-      <c r="L33" s="4" t="n"/>
-      <c r="M33" s="4" t="n"/>
-      <c r="N33" s="4" t="n"/>
-      <c r="O33" s="4" t="n"/>
-      <c r="P33" s="4" t="n"/>
-      <c r="Q33" s="4" t="n"/>
-      <c r="R33" s="4" t="n"/>
-      <c r="S33" s="4" t="n"/>
-      <c r="T33" s="4" t="n"/>
-      <c r="U33" s="4" t="n"/>
-      <c r="V33" s="4" t="n"/>
-      <c r="W33" s="4" t="n"/>
-      <c r="X33" s="4" t="n"/>
-      <c r="Y33" s="4" t="n"/>
-      <c r="Z33" s="4" t="n"/>
-      <c r="AA33" s="4" t="n"/>
-      <c r="AB33" s="4" t="n"/>
-      <c r="AC33" s="4" t="n"/>
-      <c r="AD33" s="4" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="n"/>
-      <c r="B34" s="4" t="n"/>
-      <c r="C34" s="4" t="n"/>
-      <c r="D34" s="4" t="n"/>
-      <c r="E34" s="4" t="n"/>
-      <c r="F34" s="4" t="n"/>
-      <c r="G34" s="4" t="n"/>
-      <c r="H34" s="4" t="n"/>
-      <c r="I34" s="4" t="n"/>
-      <c r="J34" s="4" t="n"/>
-      <c r="K34" s="4" t="n"/>
-      <c r="L34" s="4" t="n"/>
-      <c r="M34" s="4" t="n"/>
-      <c r="N34" s="4" t="n"/>
-      <c r="O34" s="4" t="n"/>
-      <c r="P34" s="4" t="n"/>
-      <c r="Q34" s="4" t="n"/>
-      <c r="R34" s="4" t="n"/>
-      <c r="S34" s="4" t="n"/>
-      <c r="T34" s="4" t="n"/>
-      <c r="U34" s="4" t="n"/>
-      <c r="V34" s="4" t="n"/>
-      <c r="W34" s="4" t="n"/>
-      <c r="X34" s="4" t="n"/>
-      <c r="Y34" s="4" t="n"/>
-      <c r="Z34" s="4" t="n"/>
-      <c r="AA34" s="4" t="n"/>
-      <c r="AB34" s="4" t="n"/>
-      <c r="AC34" s="4" t="n"/>
-      <c r="AD34" s="4" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="n"/>
-      <c r="B35" s="4" t="n"/>
-      <c r="C35" s="4" t="n"/>
-      <c r="D35" s="4" t="n"/>
-      <c r="E35" s="4" t="n"/>
-      <c r="F35" s="4" t="n"/>
-      <c r="G35" s="4" t="n"/>
-      <c r="H35" s="4" t="n"/>
-      <c r="I35" s="4" t="n"/>
-      <c r="J35" s="4" t="n"/>
-      <c r="K35" s="4" t="n"/>
-      <c r="L35" s="4" t="n"/>
-      <c r="M35" s="4" t="n"/>
-      <c r="N35" s="4" t="n"/>
-      <c r="O35" s="4" t="n"/>
-      <c r="P35" s="4" t="n"/>
-      <c r="Q35" s="4" t="n"/>
-      <c r="R35" s="4" t="n"/>
-      <c r="S35" s="4" t="n"/>
-      <c r="T35" s="4" t="n"/>
-      <c r="U35" s="4" t="n"/>
-      <c r="V35" s="4" t="n"/>
-      <c r="W35" s="4" t="n"/>
-      <c r="X35" s="4" t="n"/>
-      <c r="Y35" s="4" t="n"/>
-      <c r="Z35" s="4" t="n"/>
-      <c r="AA35" s="4" t="n"/>
-      <c r="AB35" s="4" t="n"/>
-      <c r="AC35" s="4" t="n"/>
-      <c r="AD35" s="4" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="n"/>
-      <c r="B36" s="4" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="4" t="n"/>
-      <c r="E36" s="4" t="n"/>
-      <c r="F36" s="4" t="n"/>
-      <c r="G36" s="4" t="n"/>
-      <c r="H36" s="4" t="n"/>
-      <c r="I36" s="4" t="n"/>
-      <c r="J36" s="4" t="n"/>
-      <c r="K36" s="4" t="n"/>
-      <c r="L36" s="4" t="n"/>
-      <c r="M36" s="4" t="n"/>
-      <c r="N36" s="4" t="n"/>
-      <c r="O36" s="4" t="n"/>
-      <c r="P36" s="4" t="n"/>
-      <c r="Q36" s="4" t="n"/>
-      <c r="R36" s="4" t="n"/>
-      <c r="S36" s="4" t="n"/>
-      <c r="T36" s="4" t="n"/>
-      <c r="U36" s="4" t="n"/>
-      <c r="V36" s="4" t="n"/>
-      <c r="W36" s="4" t="n"/>
-      <c r="X36" s="4" t="n"/>
-      <c r="Y36" s="4" t="n"/>
-      <c r="Z36" s="4" t="n"/>
-      <c r="AA36" s="4" t="n"/>
-      <c r="AB36" s="4" t="n"/>
-      <c r="AC36" s="4" t="n"/>
-      <c r="AD36" s="4" t="n"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="0" autoFilter="1" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="1" deleteRows="1" formatCells="0" formatRows="0" sort="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>